<commit_message>
Updated UE4 project, fixed testing scenario bug, security issues with installer and NSI script (will need to publish both an installer and 'update files' zip on releases now though. ADDED USER SETTINGS!!! 3% OR 10% RESPONSE TIME, GAMMA CORRECTED OR NOT, GAMMA CORRECTED OVERSHOOT, NON-PERCENT OVERSHOOT, VERBOSE SAVING OPTION FOR ALL THE DATA!!!!!
Also fixed so many bugs, added window focuesed hook which pauses the test if game isn't selected and quits the game is the board disconnects.
</commit_message>
<xml_diff>
--- a/Results Template.xlsx
+++ b/Results Template.xlsx
@@ -9,25 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7080"/>
   </bookViews>
   <sheets>
-    <sheet name="XG270QG-165-DP-FINAL-DATA-OSRTT" sheetId="1" r:id="rId1"/>
+    <sheet name="OSRTT DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Starting RGB</t>
   </si>
   <si>
     <t xml:space="preserve"> End RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Response Time (ms)</t>
   </si>
   <si>
     <t xml:space="preserve"> Overshoot RGB (%)</t>
@@ -79,6 +76,24 @@
   </si>
   <si>
     <t>On</t>
+  </si>
+  <si>
+    <t>Complete Response Time (ms)</t>
+  </si>
+  <si>
+    <t>3% / 10% Response Time (ms)</t>
+  </si>
+  <si>
+    <t>OVERSHOOT/UNDERSHOOT</t>
+  </si>
+  <si>
+    <t>COMPLETE TRANSITION TIME</t>
+  </si>
+  <si>
+    <t>3% OR 10% TRANSITION TIME</t>
+  </si>
+  <si>
+    <t>Average Complete Transition</t>
   </si>
 </sst>
 </file>
@@ -677,17 +692,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -697,20 +721,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -760,6 +784,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFB8809"/>
+      <color rgb="FF46A448"/>
+      <color rgb="FFEFAD35"/>
+      <color rgb="FF00B022"/>
       <color rgb="FFA5F27E"/>
     </mruColors>
   </colors>
@@ -1037,25 +1065,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V111"/>
+  <dimension ref="A1:W111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="5" customWidth="1"/>
-    <col min="17" max="19" width="5.140625" customWidth="1"/>
-    <col min="21" max="21" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="10" max="16" width="5.140625" customWidth="1"/>
+    <col min="17" max="17" width="5" customWidth="1"/>
+    <col min="18" max="20" width="5.140625" customWidth="1"/>
+    <col min="22" max="22" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1063,15 +1096,23 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1082,32 +1123,14 @@
         <v>1.7</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="15"/>
-      <c r="U2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="19">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>26</v>
       </c>
@@ -1118,789 +1141,849 @@
         <v>1.8</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="4">
+      <c r="I3" s="1"/>
+      <c r="J3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="12"/>
+      <c r="V3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="9">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>3.7</v>
+      </c>
+      <c r="D4">
+        <v>3.7</v>
+      </c>
+      <c r="E4">
+        <v>3.9</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K4" s="3">
         <f>B2</f>
         <v>26</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L4" s="3">
         <f>B4</f>
         <v>51</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M4" s="3">
         <f>B6</f>
         <v>77</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N4" s="3">
         <f>B8</f>
         <v>102</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O4" s="3">
         <f>B10</f>
         <v>128</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P4" s="3">
         <f>B12</f>
         <v>153</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q4" s="3">
         <f>B14</f>
         <v>179</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R4" s="3">
         <f>B16</f>
         <v>204</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S4" s="3">
         <f>B18</f>
         <v>230</v>
       </c>
-      <c r="S3" s="6">
+      <c r="T4" s="4">
         <f>B20</f>
         <v>255</v>
       </c>
-      <c r="U3" t="s">
-        <v>7</v>
-      </c>
-      <c r="V3" s="18">
-        <f>1000/V2</f>
+      <c r="V4" t="s">
+        <v>6</v>
+      </c>
+      <c r="W4" s="8">
+        <f>1000/W3</f>
         <v>6.0606060606060606</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>51</v>
       </c>
-      <c r="C4">
-        <v>3.7</v>
-      </c>
-      <c r="D4">
-        <v>3.9</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2.8</v>
+      </c>
+      <c r="D5">
+        <v>2.8</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="1">
+      <c r="J5" s="18"/>
+      <c r="K5" s="19">
         <f>C2</f>
         <v>1.7</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L5" s="19">
         <f>C4</f>
         <v>3.7</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M5" s="19">
         <f>C6</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N5" s="19">
         <f>C8</f>
         <v>3.3</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O5" s="19">
         <f>C10</f>
         <v>5</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P5" s="19">
         <f>C12</f>
         <v>3.5</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q5" s="19">
         <f>C14</f>
         <v>2.5</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R5" s="19">
         <f>C16</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S5" s="19">
         <f>C18</f>
         <v>5.7</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T5" s="20">
         <f>C20</f>
         <v>5</v>
       </c>
-      <c r="U4" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="18">
-        <f>((COUNTIF(I4:S14, "&lt;" &amp;V3))/110)*100</f>
+      <c r="V5" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" s="8">
+        <f>((COUNTIF(J5:T15, "&lt;" &amp;W4))/110)*100</f>
         <v>94.545454545454547</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>51</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>2.8</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="8">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="6">
         <f>A3</f>
         <v>26</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J6" s="19">
         <f>C3</f>
         <v>1.8</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="1">
+      <c r="K6" s="18"/>
+      <c r="L6" s="19">
         <f>C22</f>
         <v>1.9</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M6" s="19">
         <f>C24</f>
         <v>3.9</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N6" s="19">
         <f>C26</f>
         <v>2.4</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O6" s="19">
         <f>C28</f>
         <v>2.5</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P6" s="19">
         <f>C30</f>
         <v>2.5</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q6" s="19">
         <f>C32</f>
         <v>3.7</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R6" s="19">
         <f>C34</f>
         <v>5.5</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S6" s="19">
         <f>C36</f>
         <v>5.4</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T6" s="20">
         <f>C38</f>
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>77</v>
       </c>
-      <c r="C6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="8">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>3.4</v>
+      </c>
+      <c r="D7">
+        <v>3.4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="6">
         <f>A5</f>
         <v>51</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J7" s="19">
         <f>C5</f>
         <v>2.8</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K7" s="19">
         <f>C23</f>
         <v>1.6</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="1">
+      <c r="L7" s="18"/>
+      <c r="M7" s="19">
         <f>C40</f>
         <v>5</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N7" s="19">
         <f>C42</f>
         <v>4.3</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O7" s="19">
         <f>C44</f>
         <v>2.6</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P7" s="19">
         <f>C46</f>
         <v>3.6</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q7" s="19">
         <f>C48</f>
         <v>4.7</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R7" s="19">
         <f>C50</f>
         <v>5.6</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S7" s="19">
         <f>C52</f>
         <v>5.8</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T7" s="20">
         <f>C54</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="U6" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="18">
-        <f>AVERAGE(I4:S14)</f>
+      <c r="V7" t="s">
+        <v>8</v>
+      </c>
+      <c r="W7" s="23">
+        <f>AVERAGE(J5:T15)</f>
         <v>4.2936363636363621</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>77</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>3.4</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="8">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>3.3</v>
+      </c>
+      <c r="D8">
+        <v>3.3</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="6">
         <f>A7</f>
         <v>77</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J8" s="19">
         <f>C7</f>
         <v>3.4</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K8" s="19">
         <f>C25</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L8" s="19">
         <f>C41</f>
         <v>1.9</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="1">
+      <c r="M8" s="18"/>
+      <c r="N8" s="19">
         <f>C56</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O8" s="19">
         <f>C58</f>
         <v>4.8</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P8" s="19">
         <f>C60</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q8" s="19">
         <f>C62</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R8" s="19">
         <f>C64</f>
         <v>5.6</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S8" s="19">
         <f>C66</f>
         <v>5.6</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T8" s="20">
         <f>C68</f>
         <v>4.8</v>
       </c>
-      <c r="U7" t="s">
-        <v>10</v>
-      </c>
-      <c r="V7" s="18">
-        <f>AVERAGE(J4,K4:K5,L4:L6,M4:M7,N4:N8,O4:O9,P4:P10,Q4:Q11,R4:R12,S4:S13)</f>
+      <c r="V8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="23">
+        <f>AVERAGE(K5,L5:L6,M5:M7,N5:N8,O5:O9,P5:P10,Q5:Q11,R5:R12,S5:S13,T5:T14)</f>
         <v>4.5509090909090908</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>102</v>
       </c>
-      <c r="C8">
-        <v>3.3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="8">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>3.9</v>
+      </c>
+      <c r="D9">
+        <v>3.9</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="6">
         <f>A9</f>
         <v>102</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J9" s="19">
         <f>C9</f>
         <v>3.9</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K9" s="19">
         <f>C27</f>
         <v>2.4</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L9" s="19">
         <f>C43</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M9" s="19">
         <f>C57</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="1">
+      <c r="N9" s="18"/>
+      <c r="O9" s="19">
         <f>C70</f>
         <v>5.3</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P9" s="19">
         <f>C72</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q9" s="19">
         <f>C74</f>
         <v>5.3</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R9" s="19">
         <f>C76</f>
         <v>5.6</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S9" s="19">
         <f>C78</f>
         <v>5.7</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T9" s="20">
         <f>C80</f>
         <v>4.8</v>
       </c>
-      <c r="U8" t="s">
-        <v>11</v>
-      </c>
-      <c r="V8" s="18">
-        <f>AVERAGE(I5:I14,J6:J14,K7:K14,L8:L14,M9:M14,N10:N14,O11:O14,P12:P14,Q13:Q14,R14)</f>
+      <c r="V9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="23">
+        <f>AVERAGE(J6:J15,K7:K15,L8:L15,M9:M15,N10:N15,O11:O15,P12:P15,Q13:Q15,R14:R15,S15)</f>
         <v>4.0363636363636379</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>102</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>3.9</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="8">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>128</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="6">
         <f>A11</f>
         <v>128</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J10" s="19">
         <f>C11</f>
         <v>4.3</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K10" s="19">
         <f>C29</f>
         <v>2.7</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L10" s="19">
         <f>C45</f>
         <v>2.4</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M10" s="19">
         <f>C59</f>
         <v>2.5</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N10" s="19">
         <f>C71</f>
         <v>4</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="1">
+      <c r="O10" s="18"/>
+      <c r="P10" s="19">
         <f>C82</f>
         <v>5.2</v>
       </c>
-      <c r="P9" s="1">
+      <c r="Q10" s="19">
         <f>C84</f>
         <v>5.4</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R10" s="19">
         <f>C86</f>
         <v>5.7</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S10" s="19">
         <f>C88</f>
         <v>5.6</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T10" s="20">
         <f>C90</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="U9" t="s">
-        <v>12</v>
-      </c>
-      <c r="V9">
-        <f>S4+I14</f>
+      <c r="V10" t="s">
+        <v>11</v>
+      </c>
+      <c r="W10" s="24">
+        <f>T5+J15</f>
         <v>10.7</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>128</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="8">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>4.3</v>
+      </c>
+      <c r="D11">
+        <v>4.3</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="6">
         <f>A13</f>
         <v>153</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J11" s="19">
         <f>C13</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K11" s="19">
         <f>C31</f>
         <v>3.5</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L11" s="19">
         <f>C47</f>
         <v>2.8</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M11" s="19">
         <f>C61</f>
         <v>2.8</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N11" s="19">
         <f>C73</f>
         <v>2.5</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O11" s="19">
         <f>C83</f>
         <v>4.3</v>
       </c>
-      <c r="O10" s="16"/>
-      <c r="P10" s="1">
+      <c r="P11" s="18"/>
+      <c r="Q11" s="19">
         <f>C92</f>
         <v>5.4</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R11" s="19">
         <f>C94</f>
         <v>5.5</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S11" s="19">
         <f>C96</f>
         <v>5.6</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T11" s="20">
         <f>C98</f>
         <v>4.5</v>
       </c>
-      <c r="U10" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10">
-        <f>MIN(I4:S14)</f>
+      <c r="V11" t="s">
+        <v>12</v>
+      </c>
+      <c r="W11" s="24">
+        <f>MIN(J5:T15)</f>
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>128</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>4.3</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="8">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>153</v>
+      </c>
+      <c r="C12">
+        <v>3.5</v>
+      </c>
+      <c r="D12">
+        <v>3.5</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="6">
         <f>A15</f>
         <v>179</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J12" s="19">
         <f>C15</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K12" s="19">
         <f>C33</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L12" s="19">
         <f>C49</f>
         <v>2.8</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M12" s="19">
         <f>C63</f>
         <v>3.7</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N12" s="19">
         <f>C75</f>
         <v>2.9</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O12" s="19">
         <f>C85</f>
         <v>2.5</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P12" s="19">
         <f>C93</f>
         <v>4.3</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="1">
+      <c r="Q12" s="18"/>
+      <c r="R12" s="19">
         <f>C100</f>
         <v>5.4</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S12" s="19">
         <f>C102</f>
         <v>5.6</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T12" s="20">
         <f>C104</f>
         <v>4.5</v>
       </c>
-      <c r="U11" t="s">
-        <v>14</v>
-      </c>
-      <c r="V11">
-        <f>MAX(I4:S14)</f>
+      <c r="V12" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" s="24">
+        <f>MAX(J5:T15)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>153</v>
       </c>
-      <c r="C12">
-        <v>3.5</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="8">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="6">
         <f>A17</f>
         <v>204</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J13" s="19">
         <f>C17</f>
         <v>5.3</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K13" s="19">
         <f>C35</f>
         <v>5.4</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L13" s="19">
         <f>C51</f>
         <v>2.7</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M13" s="19">
         <f>C65</f>
         <v>3.9</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N13" s="19">
         <f>C77</f>
         <v>4.8</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O13" s="19">
         <f>C87</f>
         <v>2.7</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P13" s="19">
         <f>C95</f>
         <v>4.2</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q13" s="19">
         <f>C101</f>
         <v>4.3</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="1">
+      <c r="R13" s="18"/>
+      <c r="S13" s="19">
         <f>C106</f>
         <v>5.6</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T13" s="20">
         <f>C108</f>
         <v>3.9</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>153</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="8">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>179</v>
+      </c>
+      <c r="C14">
+        <v>2.5</v>
+      </c>
+      <c r="D14">
+        <v>2.5</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="6">
         <f>A19</f>
         <v>230</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J14" s="19">
         <f>C19</f>
         <v>5.4</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K14" s="19">
         <f>C37</f>
         <v>6</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L14" s="19">
         <f>C53</f>
         <v>3.5</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M14" s="19">
         <f>C67</f>
         <v>4.7</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N14" s="19">
         <f>C79</f>
         <v>5.5</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O14" s="19">
         <f>C89</f>
         <v>3.9</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P14" s="19">
         <f>C97</f>
         <v>3</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q14" s="19">
         <f>C103</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R14" s="19">
         <f>C107</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="R13" s="16"/>
-      <c r="S13" s="2">
+      <c r="S14" s="18"/>
+      <c r="T14" s="20">
         <f>C110</f>
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>179</v>
       </c>
-      <c r="C14">
-        <v>2.5</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="9">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="7">
         <f>A21</f>
         <v>255</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J15" s="21">
         <f>C21</f>
         <v>5.7</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K15" s="21">
         <f>C39</f>
         <v>6.5</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L15" s="21">
         <f>C55</f>
         <v>5.9</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M15" s="21">
         <f>C69</f>
         <v>6.6</v>
       </c>
-      <c r="M14" s="3">
+      <c r="N15" s="21">
         <f>C81</f>
         <v>5.9</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O15" s="21">
         <f>C91</f>
         <v>2.8</v>
       </c>
-      <c r="O14" s="3">
+      <c r="P15" s="21">
         <f>C99</f>
         <v>6.3</v>
       </c>
-      <c r="P14" s="3">
+      <c r="Q15" s="21">
         <f>C105</f>
         <v>6.7</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="R15" s="21">
         <f>C109</f>
         <v>7</v>
       </c>
-      <c r="R14" s="3">
+      <c r="S15" s="21">
         <f>C111</f>
         <v>6.4</v>
       </c>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>179</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T15" s="22"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1911,10 +1994,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>204</v>
       </c>
@@ -1925,10 +2011,13 @@
         <v>5.3</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5.3</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1939,10 +2028,20 @@
         <v>5.7</v>
       </c>
       <c r="D18">
+        <v>5.7</v>
+      </c>
+      <c r="E18">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>230</v>
       </c>
@@ -1953,31 +2052,13 @@
         <v>5.4</v>
       </c>
       <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
-      <c r="U19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5.4</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1988,125 +2069,104 @@
         <v>5</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="4">
-        <f>A2</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
+      <c r="I20" s="1"/>
+      <c r="J20" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="12"/>
+      <c r="V20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="W20" s="9">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>255</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>5.7</v>
+      </c>
+      <c r="D21">
+        <v>5.7</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
         <f>B2</f>
         <v>26</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L21" s="3">
         <f>B4</f>
         <v>51</v>
       </c>
-      <c r="L20" s="5">
+      <c r="M21" s="3">
         <f>B6</f>
         <v>77</v>
       </c>
-      <c r="M20" s="5">
+      <c r="N21" s="3">
         <f>B8</f>
         <v>102</v>
       </c>
-      <c r="N20" s="5">
+      <c r="O21" s="3">
         <f>B10</f>
         <v>128</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P21" s="3">
         <f>B12</f>
         <v>153</v>
       </c>
-      <c r="P20" s="5">
+      <c r="Q21" s="3">
         <f>B14</f>
         <v>179</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="R21" s="3">
         <f>B16</f>
         <v>204</v>
       </c>
-      <c r="R20" s="5">
+      <c r="S21" s="3">
         <f>B18</f>
         <v>230</v>
       </c>
-      <c r="S20" s="6">
+      <c r="T21" s="4">
         <f>B20</f>
         <v>255</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>255</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>5.7</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="7">
-        <f>A2</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="1">
-        <f>D2</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="1">
-        <f>D4</f>
-        <v>3.9</v>
-      </c>
-      <c r="L21" s="1">
-        <f>D6</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
-        <f>D8</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <f>D10</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <f>D12</f>
-        <v>0</v>
-      </c>
-      <c r="P21" s="1">
-        <f>D14</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="1">
-        <f>D16</f>
-        <v>1</v>
-      </c>
-      <c r="R21" s="1">
-        <f>D18</f>
-        <v>1.3</v>
-      </c>
-      <c r="S21" s="2">
-        <f>D20</f>
-        <v>0</v>
-      </c>
-      <c r="U21" t="s">
-        <v>15</v>
-      </c>
-      <c r="V21" s="18">
-        <f>AVERAGE(I21:S31)</f>
-        <v>0.8672727272727272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>6</v>
+      </c>
+      <c r="W21" s="8">
+        <f>1000/W20</f>
+        <v>6.0606060606060606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>26</v>
       </c>
@@ -2117,624 +2177,747 @@
         <v>1.9</v>
       </c>
       <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="5">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19">
+        <f>D2</f>
+        <v>1.7</v>
+      </c>
+      <c r="L22" s="19">
+        <f>D4</f>
+        <v>3.7</v>
+      </c>
+      <c r="M22" s="19">
+        <f>D6</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N22" s="19">
+        <f>D8</f>
+        <v>3.3</v>
+      </c>
+      <c r="O22" s="19">
+        <f>D10</f>
+        <v>5</v>
+      </c>
+      <c r="P22" s="19">
+        <f>D12</f>
+        <v>3.5</v>
+      </c>
+      <c r="Q22" s="19">
+        <f>D14</f>
+        <v>2.5</v>
+      </c>
+      <c r="R22" s="19">
+        <f>D16</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S22" s="19">
+        <f>D18</f>
+        <v>5.7</v>
+      </c>
+      <c r="T22" s="20">
+        <f>D20</f>
+        <v>5</v>
+      </c>
+      <c r="V22" t="s">
+        <v>7</v>
+      </c>
+      <c r="W22" s="8">
+        <f>((COUNTIF(J22:T32, "&lt;" &amp;W21))/110)*100</f>
+        <v>94.545454545454547</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>1.6</v>
+      </c>
+      <c r="D23">
+        <v>1.6</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="6">
         <f>A3</f>
         <v>26</v>
       </c>
-      <c r="I22" s="1">
-        <f>$D3</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="1">
+      <c r="J23" s="19">
+        <f>D3</f>
+        <v>1.8</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19">
         <f>D22</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="M23" s="19">
         <f>D24</f>
+        <v>3.9</v>
+      </c>
+      <c r="N23" s="19">
+        <f>D26</f>
+        <v>2.4</v>
+      </c>
+      <c r="O23" s="19">
+        <f>D28</f>
+        <v>2.5</v>
+      </c>
+      <c r="P23" s="19">
+        <f>D30</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q23" s="19">
+        <f>D32</f>
+        <v>3.7</v>
+      </c>
+      <c r="R23" s="19">
+        <f>D34</f>
+        <v>5.5</v>
+      </c>
+      <c r="S23" s="19">
+        <f>D36</f>
+        <v>5.4</v>
+      </c>
+      <c r="T23" s="20">
+        <f>D38</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24">
+        <v>3.9</v>
+      </c>
+      <c r="D24">
+        <v>3.9</v>
+      </c>
+      <c r="E24">
         <v>1.3</v>
       </c>
-      <c r="M22" s="1">
-        <f>D26</f>
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <f>D28</f>
-        <v>0</v>
-      </c>
-      <c r="O22" s="1">
-        <f>D30</f>
-        <v>0</v>
-      </c>
-      <c r="P22" s="1">
-        <f>D32</f>
-        <v>0.6</v>
-      </c>
-      <c r="Q22" s="1">
-        <f>D34</f>
-        <v>1</v>
-      </c>
-      <c r="R22" s="1">
-        <f>D36</f>
-        <v>1.3</v>
-      </c>
-      <c r="S22" s="2">
-        <f>D38</f>
-        <v>0</v>
-      </c>
-      <c r="U22" t="s">
-        <v>16</v>
-      </c>
-      <c r="V22">
-        <f>MAX(I21:S31)</f>
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>51</v>
-      </c>
-      <c r="B23">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>1.6</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="8">
+      <c r="H24" s="14"/>
+      <c r="I24" s="6">
         <f>A5</f>
         <v>51</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J24" s="19">
         <f>D5</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="K24" s="19">
         <f>D23</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="16"/>
-      <c r="L23" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="L24" s="18"/>
+      <c r="M24" s="19">
         <f>D40</f>
-        <v>3.9</v>
-      </c>
-      <c r="M23" s="1">
+        <v>5</v>
+      </c>
+      <c r="N24" s="19">
         <f>D42</f>
-        <v>1</v>
-      </c>
-      <c r="N23" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="O24" s="19">
         <f>D44</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="P24" s="19">
         <f>D46</f>
-        <v>0.6</v>
-      </c>
-      <c r="P23" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="Q24" s="19">
         <f>D48</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q23" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="R24" s="19">
         <f>D50</f>
-        <v>1.5</v>
-      </c>
-      <c r="R23" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="S24" s="19">
         <f>D52</f>
-        <v>1.7</v>
-      </c>
-      <c r="S23" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="T24" s="20">
         <f>D54</f>
-        <v>0</v>
-      </c>
-      <c r="U23" t="s">
-        <v>17</v>
-      </c>
-      <c r="V23" s="20">
-        <f>((COUNTIF(I21:S31, "&gt;15"))/110)*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="V24" t="s">
+        <v>24</v>
+      </c>
+      <c r="W24" s="23">
+        <f>W7</f>
+        <v>4.2936363636363621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>77</v>
+      </c>
+      <c r="B25">
         <v>26</v>
       </c>
-      <c r="B24">
-        <v>77</v>
-      </c>
-      <c r="C24">
-        <v>3.9</v>
-      </c>
-      <c r="D24">
-        <v>1.3</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="8">
+      <c r="C25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="6">
         <f>A7</f>
         <v>77</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J25" s="19">
         <f>D7</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="K25" s="19">
         <f>D25</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L25" s="19">
         <f>D41</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="M25" s="18"/>
+      <c r="N25" s="19">
         <f>D56</f>
-        <v>2</v>
-      </c>
-      <c r="N24" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O25" s="19">
         <f>D58</f>
-        <v>1.6</v>
-      </c>
-      <c r="O24" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="P25" s="19">
         <f>D60</f>
-        <v>1.3</v>
-      </c>
-      <c r="P24" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q25" s="19">
         <f>D62</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q24" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R25" s="19">
         <f>D64</f>
-        <v>1.5</v>
-      </c>
-      <c r="R24" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="S25" s="19">
         <f>D66</f>
-        <v>1.7</v>
-      </c>
-      <c r="S24" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="T25" s="20">
         <f>D68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>77</v>
-      </c>
-      <c r="B25">
+        <v>4.8</v>
+      </c>
+      <c r="V25" t="s">
+        <v>8</v>
+      </c>
+      <c r="W25" s="23">
+        <f>AVERAGE(J22:T32)</f>
+        <v>4.2936363636363621</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>26</v>
       </c>
-      <c r="C25">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="8">
+      <c r="B26">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <v>2.4</v>
+      </c>
+      <c r="D26">
+        <v>2.4</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="6">
         <f>A9</f>
         <v>102</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J26" s="19">
         <f>D9</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="K26" s="19">
         <f>D27</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="L26" s="19">
         <f>D43</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M26" s="19">
         <f>D57</f>
-        <v>2.6</v>
-      </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N26" s="18"/>
+      <c r="O26" s="19">
         <f>D70</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O25" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="P26" s="19">
         <f>D72</f>
-        <v>1.3</v>
-      </c>
-      <c r="P25" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q26" s="19">
         <f>D74</f>
-        <v>1.7</v>
-      </c>
-      <c r="Q25" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="R26" s="19">
         <f>D76</f>
-        <v>2</v>
-      </c>
-      <c r="R25" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="S26" s="19">
         <f>D78</f>
-        <v>1.7</v>
-      </c>
-      <c r="S25" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="T26" s="20">
         <f>D80</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26">
+        <v>4.8</v>
+      </c>
+      <c r="V26" t="s">
+        <v>9</v>
+      </c>
+      <c r="W26" s="23">
+        <f>AVERAGE(K22,L22:L23,M22:M24,N22:N25,O22:O26,P22:P27,Q22:Q28,R22:R29,S22:S30,T22:T31)</f>
+        <v>4.5509090909090908</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>102</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="B26">
-        <v>102</v>
-      </c>
-      <c r="C26">
+      <c r="C27">
         <v>2.4</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="8">
+      <c r="D27">
+        <v>2.4</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14"/>
+      <c r="I27" s="6">
         <f>A11</f>
         <v>128</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J27" s="19">
         <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="K27" s="19">
         <f>D29</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="L27" s="19">
         <f>D45</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="M27" s="19">
         <f>D59</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="N27" s="19">
         <f>D71</f>
-        <v>1</v>
-      </c>
-      <c r="N26" s="16"/>
-      <c r="O26" s="1">
+        <v>4</v>
+      </c>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19">
         <f>D82</f>
-        <v>2</v>
-      </c>
-      <c r="P26" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="Q27" s="19">
         <f>D84</f>
-        <v>1.7</v>
-      </c>
-      <c r="Q26" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="R27" s="19">
         <f>D86</f>
-        <v>2</v>
-      </c>
-      <c r="R26" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="S27" s="19">
         <f>D88</f>
-        <v>1.7</v>
-      </c>
-      <c r="S26" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="T27" s="20">
         <f>D90</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>102</v>
-      </c>
-      <c r="B27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V27" t="s">
+        <v>10</v>
+      </c>
+      <c r="W27" s="23">
+        <f>AVERAGE(J23:J32,K24:K32,L25:L32,M26:M32,N27:N32,O28:O32,P29:P32,Q30:Q32,R31:R32,S32)</f>
+        <v>4.0363636363636379</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>2.4</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="8">
+      <c r="B28">
+        <v>128</v>
+      </c>
+      <c r="C28">
+        <v>2.5</v>
+      </c>
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="6">
         <f>A13</f>
         <v>153</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J28" s="19">
         <f>D13</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K28" s="19">
         <f>D31</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="L28" s="19">
         <f>D47</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="M28" s="19">
         <f>D61</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="N28" s="19">
         <f>D73</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="O28" s="19">
         <f>D83</f>
-        <v>1.6</v>
-      </c>
-      <c r="O27" s="16"/>
-      <c r="P27" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="19">
         <f>D92</f>
-        <v>1.7</v>
-      </c>
-      <c r="Q27" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="R28" s="19">
         <f>D94</f>
-        <v>2</v>
-      </c>
-      <c r="R27" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="S28" s="19">
         <f>D96</f>
-        <v>1.7</v>
-      </c>
-      <c r="S27" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="T28" s="20">
         <f>D98</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <v>4.5</v>
+      </c>
+      <c r="V28" t="s">
+        <v>11</v>
+      </c>
+      <c r="W28" s="24">
+        <f>T22+J32</f>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>128</v>
+      </c>
+      <c r="B29">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>128</v>
-      </c>
-      <c r="C28">
-        <v>2.5</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="8">
+      <c r="C29">
+        <v>2.7</v>
+      </c>
+      <c r="D29">
+        <v>2.7</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="6">
         <f>A15</f>
         <v>179</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J29" s="19">
         <f>D15</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K29" s="19">
         <f>D33</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L29" s="19">
         <f>D49</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="M29" s="19">
         <f>D63</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="N29" s="19">
         <f>D75</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="O29" s="19">
         <f>D85</f>
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="P29" s="19">
         <f>D93</f>
-        <v>1.3</v>
-      </c>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="19">
         <f>D100</f>
-        <v>2</v>
-      </c>
-      <c r="R28" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="S29" s="19">
         <f>D102</f>
-        <v>1.7</v>
-      </c>
-      <c r="S28" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="T29" s="20">
         <f>D104</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>128</v>
-      </c>
-      <c r="B29">
+        <v>4.5</v>
+      </c>
+      <c r="V29" t="s">
+        <v>12</v>
+      </c>
+      <c r="W29" s="24">
+        <f>MIN(J22:T32)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>26</v>
       </c>
-      <c r="C29">
-        <v>2.7</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="8">
+      <c r="B30">
+        <v>153</v>
+      </c>
+      <c r="C30">
+        <v>2.5</v>
+      </c>
+      <c r="D30">
+        <v>2.5</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="6">
         <f>A17</f>
         <v>204</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J30" s="19">
         <f>D17</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="K30" s="19">
         <f>D35</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="L30" s="19">
         <f>D51</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="M30" s="19">
         <f>D65</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="N30" s="19">
         <f>D77</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="O30" s="19">
         <f>D87</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="P30" s="19">
         <f>D95</f>
-        <v>0.6</v>
-      </c>
-      <c r="P29" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="Q30" s="19">
         <f>D101</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="R30" s="18"/>
+      <c r="S30" s="19">
         <f>D106</f>
-        <v>1.7</v>
-      </c>
-      <c r="S29" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="T30" s="20">
         <f>D108</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30">
+        <v>3.9</v>
+      </c>
+      <c r="V30" t="s">
+        <v>13</v>
+      </c>
+      <c r="W30" s="24">
+        <f>MAX(J22:T32)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>153</v>
+      </c>
+      <c r="B31">
         <v>26</v>
       </c>
-      <c r="B30">
-        <v>153</v>
-      </c>
-      <c r="C30">
-        <v>2.5</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="8">
+      <c r="C31">
+        <v>3.5</v>
+      </c>
+      <c r="D31">
+        <v>3.5</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="6">
         <f>A19</f>
         <v>230</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J31" s="19">
         <f>D19</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="K31" s="19">
         <f>D37</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="1">
+        <v>6</v>
+      </c>
+      <c r="L31" s="19">
         <f>D53</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="M31" s="19">
         <f>D67</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="N31" s="19">
         <f>D79</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="O31" s="19">
         <f>D89</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="P31" s="19">
         <f>D97</f>
-        <v>0</v>
-      </c>
-      <c r="P30" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="19">
         <f>D103</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R31" s="19">
+        <f>D107</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S31" s="18"/>
+      <c r="T31" s="20">
+        <f>D110</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>179</v>
+      </c>
+      <c r="C32">
+        <v>3.7</v>
+      </c>
+      <c r="D32">
+        <v>3.7</v>
+      </c>
+      <c r="E32">
         <v>0.6</v>
       </c>
-      <c r="Q30" s="1">
-        <f>D107</f>
-        <v>1</v>
-      </c>
-      <c r="R30" s="16"/>
-      <c r="S30" s="2">
-        <f>D110</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>153</v>
-      </c>
-      <c r="B31">
-        <v>26</v>
-      </c>
-      <c r="C31">
-        <v>3.5</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="9">
+      <c r="H32" s="15"/>
+      <c r="I32" s="7">
         <f>A21</f>
         <v>255</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J32" s="21">
         <f>D21</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="K32" s="21">
         <f>D39</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="L32" s="21">
         <f>D55</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="M32" s="21">
         <f>D69</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="N32" s="21">
         <f>D81</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="O32" s="21">
         <f>D91</f>
-        <v>0</v>
-      </c>
-      <c r="O31" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="P32" s="21">
         <f>D99</f>
-        <v>5</v>
-      </c>
-      <c r="P31" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="Q32" s="21">
         <f>D105</f>
-        <v>6.8</v>
-      </c>
-      <c r="Q31" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="R32" s="21">
         <f>D109</f>
-        <v>10.6</v>
-      </c>
-      <c r="R31" s="3">
+        <v>7</v>
+      </c>
+      <c r="S32" s="21">
         <f>D111</f>
-        <v>6.6</v>
-      </c>
-      <c r="S31" s="17"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>26</v>
-      </c>
-      <c r="B32">
-        <v>179</v>
-      </c>
-      <c r="C32">
-        <v>3.7</v>
-      </c>
-      <c r="D32">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.4</v>
+      </c>
+      <c r="T32" s="22"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>179</v>
       </c>
@@ -2745,10 +2928,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -2759,10 +2945,20 @@
         <v>5.5</v>
       </c>
       <c r="D34">
+        <v>5.5</v>
+      </c>
+      <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H34" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+    </row>
+    <row r="35" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>204</v>
       </c>
@@ -2773,10 +2969,13 @@
         <v>5.4</v>
       </c>
       <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>26</v>
       </c>
@@ -2787,10 +2986,34 @@
         <v>5.4</v>
       </c>
       <c r="D36">
+        <v>5.4</v>
+      </c>
+      <c r="E36">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="12"/>
+      <c r="V36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W36" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>230</v>
       </c>
@@ -2801,10 +3024,59 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="2">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <f>B2</f>
+        <v>26</v>
+      </c>
+      <c r="L37" s="3">
+        <f>B4</f>
+        <v>51</v>
+      </c>
+      <c r="M37" s="3">
+        <f>B6</f>
+        <v>77</v>
+      </c>
+      <c r="N37" s="3">
+        <f>B8</f>
+        <v>102</v>
+      </c>
+      <c r="O37" s="3">
+        <f>B10</f>
+        <v>128</v>
+      </c>
+      <c r="P37" s="3">
+        <f>B12</f>
+        <v>153</v>
+      </c>
+      <c r="Q37" s="3">
+        <f>B14</f>
+        <v>179</v>
+      </c>
+      <c r="R37" s="3">
+        <f>B16</f>
+        <v>204</v>
+      </c>
+      <c r="S37" s="3">
+        <f>B18</f>
+        <v>230</v>
+      </c>
+      <c r="T37" s="4">
+        <f>B20</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>26</v>
       </c>
@@ -2815,10 +3087,68 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="5">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="K38" s="19">
+        <f>E2</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="19">
+        <f>E4</f>
+        <v>3.9</v>
+      </c>
+      <c r="M38" s="19">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="19">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="19">
+        <f>E10</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="19">
+        <f>E12</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="19">
+        <f>E14</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="19">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="S38" s="19">
+        <f>E18</f>
+        <v>1.3</v>
+      </c>
+      <c r="T38" s="20">
+        <f>E20</f>
+        <v>0</v>
+      </c>
+      <c r="V38" t="s">
+        <v>14</v>
+      </c>
+      <c r="W38" s="23">
+        <f>AVERAGE(J38:T48)</f>
+        <v>0.8672727272727272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>255</v>
       </c>
@@ -2829,10 +3159,66 @@
         <v>6.5</v>
       </c>
       <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.5</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="H39" s="14"/>
+      <c r="I39" s="6">
+        <f>A3</f>
+        <v>26</v>
+      </c>
+      <c r="J39" s="19">
+        <f>$E3</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="18"/>
+      <c r="L39" s="19">
+        <f>E22</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="19">
+        <f>E24</f>
+        <v>1.3</v>
+      </c>
+      <c r="N39" s="19">
+        <f>E26</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="19">
+        <f>E28</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="19">
+        <f>E30</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="19">
+        <f>E32</f>
+        <v>0.6</v>
+      </c>
+      <c r="R39" s="19">
+        <f>E34</f>
+        <v>1</v>
+      </c>
+      <c r="S39" s="19">
+        <f>E36</f>
+        <v>1.3</v>
+      </c>
+      <c r="T39" s="20">
+        <f>E38</f>
+        <v>0</v>
+      </c>
+      <c r="V39" t="s">
+        <v>15</v>
+      </c>
+      <c r="W39" s="24">
+        <f>MAX(J38:T48)</f>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>51</v>
       </c>
@@ -2843,10 +3229,66 @@
         <v>5</v>
       </c>
       <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H40" s="14"/>
+      <c r="I40" s="6">
+        <f>A5</f>
+        <v>51</v>
+      </c>
+      <c r="J40" s="19">
+        <f>E5</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="19">
+        <f>E23</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="18"/>
+      <c r="M40" s="19">
+        <f>E40</f>
+        <v>3.9</v>
+      </c>
+      <c r="N40" s="19">
+        <f>E42</f>
+        <v>1</v>
+      </c>
+      <c r="O40" s="19">
+        <f>E44</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="19">
+        <f>E46</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q40" s="19">
+        <f>E48</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R40" s="19">
+        <f>E50</f>
+        <v>1.5</v>
+      </c>
+      <c r="S40" s="19">
+        <f>E52</f>
+        <v>1.7</v>
+      </c>
+      <c r="T40" s="20">
+        <f>E54</f>
+        <v>0</v>
+      </c>
+      <c r="V40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W40" s="25">
+        <f>((COUNTIF(J38:T48, "&gt;15"))/110)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>77</v>
       </c>
@@ -2857,10 +3299,59 @@
         <v>1.9</v>
       </c>
       <c r="D41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="14"/>
+      <c r="I41" s="6">
+        <f>A7</f>
+        <v>77</v>
+      </c>
+      <c r="J41" s="19">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="K41" s="19">
+        <f>E25</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="19">
+        <f>E41</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="18"/>
+      <c r="N41" s="19">
+        <f>E56</f>
+        <v>2</v>
+      </c>
+      <c r="O41" s="19">
+        <f>E58</f>
+        <v>1.6</v>
+      </c>
+      <c r="P41" s="19">
+        <f>E60</f>
+        <v>1.3</v>
+      </c>
+      <c r="Q41" s="19">
+        <f>E62</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R41" s="19">
+        <f>E64</f>
+        <v>1.5</v>
+      </c>
+      <c r="S41" s="19">
+        <f>E66</f>
+        <v>1.7</v>
+      </c>
+      <c r="T41" s="20">
+        <f>E68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>51</v>
       </c>
@@ -2871,10 +3362,59 @@
         <v>4.3</v>
       </c>
       <c r="D42">
+        <v>4.3</v>
+      </c>
+      <c r="E42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H42" s="14"/>
+      <c r="I42" s="6">
+        <f>A9</f>
+        <v>102</v>
+      </c>
+      <c r="J42" s="19">
+        <f>E9</f>
+        <v>0</v>
+      </c>
+      <c r="K42" s="19">
+        <f>E27</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="19">
+        <f>E43</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="19">
+        <f>E57</f>
+        <v>2.6</v>
+      </c>
+      <c r="N42" s="18"/>
+      <c r="O42" s="19">
+        <f>E70</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P42" s="19">
+        <f>E72</f>
+        <v>1.3</v>
+      </c>
+      <c r="Q42" s="19">
+        <f>E74</f>
+        <v>1.7</v>
+      </c>
+      <c r="R42" s="19">
+        <f>E76</f>
+        <v>2</v>
+      </c>
+      <c r="S42" s="19">
+        <f>E78</f>
+        <v>1.7</v>
+      </c>
+      <c r="T42" s="20">
+        <f>E80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>102</v>
       </c>
@@ -2885,10 +3425,59 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="H43" s="14"/>
+      <c r="I43" s="6">
+        <f>A11</f>
+        <v>128</v>
+      </c>
+      <c r="J43" s="19">
+        <f>E11</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="19">
+        <f>E29</f>
+        <v>0</v>
+      </c>
+      <c r="L43" s="19">
+        <f>E45</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="19">
+        <f>E59</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="19">
+        <f>E71</f>
+        <v>1</v>
+      </c>
+      <c r="O43" s="18"/>
+      <c r="P43" s="19">
+        <f>E82</f>
+        <v>2</v>
+      </c>
+      <c r="Q43" s="19">
+        <f>E84</f>
+        <v>1.7</v>
+      </c>
+      <c r="R43" s="19">
+        <f>E86</f>
+        <v>2</v>
+      </c>
+      <c r="S43" s="19">
+        <f>E88</f>
+        <v>1.7</v>
+      </c>
+      <c r="T43" s="20">
+        <f>E90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>51</v>
       </c>
@@ -2899,10 +3488,59 @@
         <v>2.6</v>
       </c>
       <c r="D44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.6</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="H44" s="14"/>
+      <c r="I44" s="6">
+        <f>A13</f>
+        <v>153</v>
+      </c>
+      <c r="J44" s="19">
+        <f>E13</f>
+        <v>0</v>
+      </c>
+      <c r="K44" s="19">
+        <f>E31</f>
+        <v>0</v>
+      </c>
+      <c r="L44" s="19">
+        <f>E47</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="19">
+        <f>E61</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="19">
+        <f>E73</f>
+        <v>0</v>
+      </c>
+      <c r="O44" s="19">
+        <f>E83</f>
+        <v>1.6</v>
+      </c>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="19">
+        <f>E92</f>
+        <v>1.7</v>
+      </c>
+      <c r="R44" s="19">
+        <f>E94</f>
+        <v>2</v>
+      </c>
+      <c r="S44" s="19">
+        <f>E96</f>
+        <v>1.7</v>
+      </c>
+      <c r="T44" s="20">
+        <f>E98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>128</v>
       </c>
@@ -2913,10 +3551,59 @@
         <v>2.4</v>
       </c>
       <c r="D45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.4</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="14"/>
+      <c r="I45" s="6">
+        <f>A15</f>
+        <v>179</v>
+      </c>
+      <c r="J45" s="19">
+        <f>E15</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="19">
+        <f>E33</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="19">
+        <f>E49</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="19">
+        <f>E63</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="19">
+        <f>E75</f>
+        <v>0</v>
+      </c>
+      <c r="O45" s="19">
+        <f>E85</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="19">
+        <f>E93</f>
+        <v>1.3</v>
+      </c>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="19">
+        <f>E100</f>
+        <v>2</v>
+      </c>
+      <c r="S45" s="19">
+        <f>E102</f>
+        <v>1.7</v>
+      </c>
+      <c r="T45" s="20">
+        <f>E104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>51</v>
       </c>
@@ -2927,10 +3614,59 @@
         <v>3.6</v>
       </c>
       <c r="D46">
+        <v>3.6</v>
+      </c>
+      <c r="E46">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H46" s="14"/>
+      <c r="I46" s="6">
+        <f>A17</f>
+        <v>204</v>
+      </c>
+      <c r="J46" s="19">
+        <f>E17</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="19">
+        <f>E35</f>
+        <v>0</v>
+      </c>
+      <c r="L46" s="19">
+        <f>E51</f>
+        <v>0</v>
+      </c>
+      <c r="M46" s="19">
+        <f>E65</f>
+        <v>0</v>
+      </c>
+      <c r="N46" s="19">
+        <f>E77</f>
+        <v>0</v>
+      </c>
+      <c r="O46" s="19">
+        <f>E87</f>
+        <v>0</v>
+      </c>
+      <c r="P46" s="19">
+        <f>E95</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q46" s="19">
+        <f>E101</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R46" s="18"/>
+      <c r="S46" s="19">
+        <f>E106</f>
+        <v>1.7</v>
+      </c>
+      <c r="T46" s="20">
+        <f>E108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>153</v>
       </c>
@@ -2941,10 +3677,59 @@
         <v>2.8</v>
       </c>
       <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="H47" s="14"/>
+      <c r="I47" s="6">
+        <f>A19</f>
+        <v>230</v>
+      </c>
+      <c r="J47" s="19">
+        <f>E19</f>
+        <v>0</v>
+      </c>
+      <c r="K47" s="19">
+        <f>E37</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="19">
+        <f>E53</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="19">
+        <f>E67</f>
+        <v>0</v>
+      </c>
+      <c r="N47" s="19">
+        <f>E79</f>
+        <v>0</v>
+      </c>
+      <c r="O47" s="19">
+        <f>E89</f>
+        <v>0</v>
+      </c>
+      <c r="P47" s="19">
+        <f>E97</f>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="19">
+        <f>E103</f>
+        <v>0.6</v>
+      </c>
+      <c r="R47" s="19">
+        <f>E107</f>
+        <v>1</v>
+      </c>
+      <c r="S47" s="18"/>
+      <c r="T47" s="20">
+        <f>E110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>51</v>
       </c>
@@ -2955,10 +3740,59 @@
         <v>4.7</v>
       </c>
       <c r="D48">
+        <v>4.7</v>
+      </c>
+      <c r="E48">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H48" s="15"/>
+      <c r="I48" s="7">
+        <f>A21</f>
+        <v>255</v>
+      </c>
+      <c r="J48" s="21">
+        <f>E21</f>
+        <v>0</v>
+      </c>
+      <c r="K48" s="21">
+        <f>E39</f>
+        <v>0</v>
+      </c>
+      <c r="L48" s="21">
+        <f>E55</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="21">
+        <f>E69</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="21">
+        <f>E81</f>
+        <v>0</v>
+      </c>
+      <c r="O48" s="21">
+        <f>E91</f>
+        <v>0</v>
+      </c>
+      <c r="P48" s="21">
+        <f>E99</f>
+        <v>5</v>
+      </c>
+      <c r="Q48" s="21">
+        <f>E105</f>
+        <v>6.8</v>
+      </c>
+      <c r="R48" s="21">
+        <f>E109</f>
+        <v>10.6</v>
+      </c>
+      <c r="S48" s="21">
+        <f>E111</f>
+        <v>6.6</v>
+      </c>
+      <c r="T48" s="22"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>179</v>
       </c>
@@ -2969,10 +3803,13 @@
         <v>2.8</v>
       </c>
       <c r="D49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>51</v>
       </c>
@@ -2983,10 +3820,13 @@
         <v>5.6</v>
       </c>
       <c r="D50">
+        <v>5.6</v>
+      </c>
+      <c r="E50">
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>204</v>
       </c>
@@ -2997,10 +3837,13 @@
         <v>2.7</v>
       </c>
       <c r="D51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.7</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3011,10 +3854,13 @@
         <v>5.8</v>
       </c>
       <c r="D52">
+        <v>5.8</v>
+      </c>
+      <c r="E52">
         <v>1.7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>230</v>
       </c>
@@ -3025,10 +3871,13 @@
         <v>3.5</v>
       </c>
       <c r="D53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -3039,10 +3888,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>255</v>
       </c>
@@ -3053,10 +3905,13 @@
         <v>5.9</v>
       </c>
       <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.9</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>77</v>
       </c>
@@ -3067,10 +3922,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D56">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>102</v>
       </c>
@@ -3081,10 +3939,13 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D57">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E57">
         <v>2.6</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>77</v>
       </c>
@@ -3095,10 +3956,13 @@
         <v>4.8</v>
       </c>
       <c r="D58">
+        <v>4.8</v>
+      </c>
+      <c r="E58">
         <v>1.6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>128</v>
       </c>
@@ -3109,10 +3973,13 @@
         <v>2.5</v>
       </c>
       <c r="D59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>77</v>
       </c>
@@ -3123,10 +3990,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D60">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E60">
         <v>1.3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>153</v>
       </c>
@@ -3137,10 +4007,13 @@
         <v>2.8</v>
       </c>
       <c r="D61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>77</v>
       </c>
@@ -3151,10 +4024,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D62">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E62">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>179</v>
       </c>
@@ -3165,10 +4041,13 @@
         <v>3.7</v>
       </c>
       <c r="D63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.7</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>77</v>
       </c>
@@ -3179,10 +4058,13 @@
         <v>5.6</v>
       </c>
       <c r="D64">
+        <v>5.6</v>
+      </c>
+      <c r="E64">
         <v>1.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>204</v>
       </c>
@@ -3193,10 +4075,13 @@
         <v>3.9</v>
       </c>
       <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.9</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>77</v>
       </c>
@@ -3207,10 +4092,13 @@
         <v>5.6</v>
       </c>
       <c r="D66">
+        <v>5.6</v>
+      </c>
+      <c r="E66">
         <v>1.7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>230</v>
       </c>
@@ -3221,10 +4109,13 @@
         <v>4.7</v>
       </c>
       <c r="D67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.7</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>77</v>
       </c>
@@ -3235,10 +4126,13 @@
         <v>4.8</v>
       </c>
       <c r="D68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>255</v>
       </c>
@@ -3249,10 +4143,13 @@
         <v>6.6</v>
       </c>
       <c r="D69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.6</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>102</v>
       </c>
@@ -3263,10 +4160,13 @@
         <v>5.3</v>
       </c>
       <c r="D70">
+        <v>5.3</v>
+      </c>
+      <c r="E70">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>128</v>
       </c>
@@ -3277,10 +4177,13 @@
         <v>4</v>
       </c>
       <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>102</v>
       </c>
@@ -3291,10 +4194,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D72">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E72">
         <v>1.3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>153</v>
       </c>
@@ -3305,10 +4211,13 @@
         <v>2.5</v>
       </c>
       <c r="D73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>102</v>
       </c>
@@ -3319,10 +4228,13 @@
         <v>5.3</v>
       </c>
       <c r="D74">
+        <v>5.3</v>
+      </c>
+      <c r="E74">
         <v>1.7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>179</v>
       </c>
@@ -3333,10 +4245,13 @@
         <v>2.9</v>
       </c>
       <c r="D75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.9</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>102</v>
       </c>
@@ -3347,10 +4262,13 @@
         <v>5.6</v>
       </c>
       <c r="D76">
+        <v>5.6</v>
+      </c>
+      <c r="E76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>204</v>
       </c>
@@ -3361,10 +4279,13 @@
         <v>4.8</v>
       </c>
       <c r="D77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>102</v>
       </c>
@@ -3375,10 +4296,13 @@
         <v>5.7</v>
       </c>
       <c r="D78">
+        <v>5.7</v>
+      </c>
+      <c r="E78">
         <v>1.7</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>230</v>
       </c>
@@ -3389,10 +4313,13 @@
         <v>5.5</v>
       </c>
       <c r="D79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>102</v>
       </c>
@@ -3403,10 +4330,13 @@
         <v>4.8</v>
       </c>
       <c r="D80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>255</v>
       </c>
@@ -3417,10 +4347,13 @@
         <v>5.9</v>
       </c>
       <c r="D81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.9</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>128</v>
       </c>
@@ -3431,10 +4364,13 @@
         <v>5.2</v>
       </c>
       <c r="D82">
+        <v>5.2</v>
+      </c>
+      <c r="E82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>153</v>
       </c>
@@ -3445,10 +4381,13 @@
         <v>4.3</v>
       </c>
       <c r="D83">
+        <v>4.3</v>
+      </c>
+      <c r="E83">
         <v>1.6</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>128</v>
       </c>
@@ -3459,10 +4398,13 @@
         <v>5.4</v>
       </c>
       <c r="D84">
+        <v>5.4</v>
+      </c>
+      <c r="E84">
         <v>1.7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>179</v>
       </c>
@@ -3473,10 +4415,13 @@
         <v>2.5</v>
       </c>
       <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>128</v>
       </c>
@@ -3487,10 +4432,13 @@
         <v>5.7</v>
       </c>
       <c r="D86">
+        <v>5.7</v>
+      </c>
+      <c r="E86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>204</v>
       </c>
@@ -3501,10 +4449,13 @@
         <v>2.7</v>
       </c>
       <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.7</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>128</v>
       </c>
@@ -3515,10 +4466,13 @@
         <v>5.6</v>
       </c>
       <c r="D88">
+        <v>5.6</v>
+      </c>
+      <c r="E88">
         <v>1.7</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>230</v>
       </c>
@@ -3529,10 +4483,13 @@
         <v>3.9</v>
       </c>
       <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.9</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>128</v>
       </c>
@@ -3543,10 +4500,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>255</v>
       </c>
@@ -3557,10 +4517,13 @@
         <v>2.8</v>
       </c>
       <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>153</v>
       </c>
@@ -3571,10 +4534,13 @@
         <v>5.4</v>
       </c>
       <c r="D92">
+        <v>5.4</v>
+      </c>
+      <c r="E92">
         <v>1.7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>179</v>
       </c>
@@ -3585,10 +4551,13 @@
         <v>4.3</v>
       </c>
       <c r="D93">
+        <v>4.3</v>
+      </c>
+      <c r="E93">
         <v>1.3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>153</v>
       </c>
@@ -3599,10 +4568,13 @@
         <v>5.5</v>
       </c>
       <c r="D94">
+        <v>5.5</v>
+      </c>
+      <c r="E94">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>204</v>
       </c>
@@ -3613,10 +4585,13 @@
         <v>4.2</v>
       </c>
       <c r="D95">
+        <v>4.2</v>
+      </c>
+      <c r="E95">
         <v>0.6</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>153</v>
       </c>
@@ -3627,10 +4602,13 @@
         <v>5.6</v>
       </c>
       <c r="D96">
+        <v>5.6</v>
+      </c>
+      <c r="E96">
         <v>1.7</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>230</v>
       </c>
@@ -3641,10 +4619,13 @@
         <v>3</v>
       </c>
       <c r="D97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>153</v>
       </c>
@@ -3655,10 +4636,13 @@
         <v>4.5</v>
       </c>
       <c r="D98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>255</v>
       </c>
@@ -3669,10 +4653,13 @@
         <v>6.3</v>
       </c>
       <c r="D99">
+        <v>6.3</v>
+      </c>
+      <c r="E99">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>179</v>
       </c>
@@ -3683,10 +4670,13 @@
         <v>5.4</v>
       </c>
       <c r="D100">
+        <v>5.4</v>
+      </c>
+      <c r="E100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>204</v>
       </c>
@@ -3697,10 +4687,13 @@
         <v>4.3</v>
       </c>
       <c r="D101">
+        <v>4.3</v>
+      </c>
+      <c r="E101">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>179</v>
       </c>
@@ -3711,10 +4704,13 @@
         <v>5.6</v>
       </c>
       <c r="D102">
+        <v>5.6</v>
+      </c>
+      <c r="E102">
         <v>1.7</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>230</v>
       </c>
@@ -3725,10 +4721,13 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D103">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E103">
         <v>0.6</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>179</v>
       </c>
@@ -3739,10 +4738,13 @@
         <v>4.5</v>
       </c>
       <c r="D104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>255</v>
       </c>
@@ -3753,10 +4755,13 @@
         <v>6.7</v>
       </c>
       <c r="D105">
+        <v>6.7</v>
+      </c>
+      <c r="E105">
         <v>6.8</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>204</v>
       </c>
@@ -3767,10 +4772,13 @@
         <v>5.6</v>
       </c>
       <c r="D106">
+        <v>5.6</v>
+      </c>
+      <c r="E106">
         <v>1.7</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>230</v>
       </c>
@@ -3781,10 +4789,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D107">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>204</v>
       </c>
@@ -3795,10 +4806,13 @@
         <v>3.9</v>
       </c>
       <c r="D108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.9</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>255</v>
       </c>
@@ -3809,10 +4823,13 @@
         <v>7</v>
       </c>
       <c r="D109">
+        <v>7</v>
+      </c>
+      <c r="E109">
         <v>10.6</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>230</v>
       </c>
@@ -3823,10 +4840,13 @@
         <v>3.6</v>
       </c>
       <c r="D110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.6</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>255</v>
       </c>
@@ -3837,30 +4857,38 @@
         <v>6.4</v>
       </c>
       <c r="D111">
+        <v>6.4</v>
+      </c>
+      <c r="E111">
         <v>6.6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I19:S19"/>
-    <mergeCell ref="G21:G31"/>
-    <mergeCell ref="G4:G14"/>
-    <mergeCell ref="I2:S2"/>
+  <mergeCells count="9">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="J20:T20"/>
+    <mergeCell ref="H22:H32"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="J36:T36"/>
+    <mergeCell ref="H38:H48"/>
+    <mergeCell ref="H5:H15"/>
+    <mergeCell ref="J3:T3"/>
+    <mergeCell ref="H34:L34"/>
   </mergeCells>
-  <conditionalFormatting sqref="I4:S14">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="J5:T15 W7:W9 W24:W27 J22:T32 W11:W12 W29:W30">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="formula" val="$V$3/2"/>
-        <cfvo type="formula" val="$V$3+1"/>
-        <cfvo type="formula" val="$V$3+($V$3/2)"/>
-        <color theme="9"/>
-        <color theme="5"/>
+        <cfvo type="formula" val="$W$4/2"/>
+        <cfvo type="formula" val="$W$4+2"/>
+        <cfvo type="formula" val="$W$4*2"/>
+        <color rgb="FF46A448"/>
+        <color rgb="FFFB8809"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:S31">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="J38:T48 W38:W40">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="10"/>
@@ -3871,6 +4899,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="W28 W10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="formula" val="($W$21*2)-$W$21"/>
+        <cfvo type="formula" val="($W$21*2)+3"/>
+        <cfvo type="formula" val="$W$21*3"/>
+        <color rgb="FF46A448"/>
+        <color rgb="FFFB8809"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W22 W5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="95"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF46A448"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Final set of changes before publishing V1.0... maybe. New PCB design, new USB voltage and brightness stability checks, new settings and updates to results template.
</commit_message>
<xml_diff>
--- a/Results Template.xlsx
+++ b/Results Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\$Current Projects\Response Time Tool\OSRTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\$Current Projects\Response Time Tool\OSRTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,12 +22,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Starting RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> End RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Overshoot RGB (%)</t>
   </si>
   <si>
     <t>To / End</t>
@@ -81,9 +75,6 @@
     <t>Complete Response Time (ms)</t>
   </si>
   <si>
-    <t>3% / 10% Response Time (ms)</t>
-  </si>
-  <si>
     <t>OVERSHOOT/UNDERSHOOT</t>
   </si>
   <si>
@@ -94,6 +85,15 @@
   </si>
   <si>
     <t>Average Complete Transition</t>
+  </si>
+  <si>
+    <t>End RGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3% Response Time (ms)</t>
+  </si>
+  <si>
+    <t>Overshoot (RGB)</t>
   </si>
 </sst>
 </file>
@@ -703,6 +703,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,29 +729,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,16 +1068,11 @@
   <dimension ref="A1:W111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" customWidth="1"/>
@@ -1093,24 +1088,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -1120,10 +1115,10 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="D2">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1138,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1.8</v>
+        <v>0.6</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1149,21 +1144,21 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="23"/>
+      <c r="V3" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="12"/>
-      <c r="V3" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="W3" s="9">
         <v>165</v>
@@ -1177,13 +1172,13 @@
         <v>51</v>
       </c>
       <c r="C4">
-        <v>3.7</v>
+        <v>2.4</v>
       </c>
       <c r="D4">
-        <v>3.7</v>
+        <v>2.1</v>
       </c>
       <c r="E4">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1232,7 +1227,7 @@
         <v>255</v>
       </c>
       <c r="V4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W4" s="8">
         <f>1000/W3</f>
@@ -1247,68 +1242,68 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>2.8</v>
+        <v>1.8</v>
       </c>
       <c r="D5">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>4</v>
+      <c r="H5" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="I5" s="5">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19">
-        <f>C2</f>
-        <v>1.7</v>
-      </c>
-      <c r="L5" s="19">
-        <f>C4</f>
-        <v>3.7</v>
-      </c>
-      <c r="M5" s="19">
-        <f>C6</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N5" s="19">
-        <f>C8</f>
-        <v>3.3</v>
-      </c>
-      <c r="O5" s="19">
-        <f>C10</f>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11">
+        <f>$C2</f>
+        <v>1.6</v>
+      </c>
+      <c r="L5" s="11">
+        <f>$C4</f>
+        <v>2.4</v>
+      </c>
+      <c r="M5" s="11">
+        <f>$C6</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N5" s="11">
+        <f>$C8</f>
+        <v>4.7</v>
+      </c>
+      <c r="O5" s="11">
+        <f>$C10</f>
+        <v>5.2</v>
+      </c>
+      <c r="P5" s="11">
+        <f>$C12</f>
+        <v>4.5</v>
+      </c>
+      <c r="Q5" s="11">
+        <f>$C14</f>
+        <v>3.1</v>
+      </c>
+      <c r="R5" s="11">
+        <f>$C16</f>
+        <v>4.8</v>
+      </c>
+      <c r="S5" s="11">
+        <f>$C18</f>
+        <v>5.5</v>
+      </c>
+      <c r="T5" s="12">
+        <f>$C20</f>
+        <v>5.9</v>
+      </c>
+      <c r="V5" t="s">
         <v>5</v>
-      </c>
-      <c r="P5" s="19">
-        <f>C12</f>
-        <v>3.5</v>
-      </c>
-      <c r="Q5" s="19">
-        <f>C14</f>
-        <v>2.5</v>
-      </c>
-      <c r="R5" s="19">
-        <f>C16</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="S5" s="19">
-        <f>C18</f>
-        <v>5.7</v>
-      </c>
-      <c r="T5" s="20">
-        <f>C20</f>
-        <v>5</v>
-      </c>
-      <c r="V5" t="s">
-        <v>7</v>
       </c>
       <c r="W5" s="8">
         <f>((COUNTIF(J5:T15, "&lt;" &amp;W4))/110)*100</f>
-        <v>94.545454545454547</v>
+        <v>81.818181818181827</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1319,59 +1314,59 @@
         <v>77</v>
       </c>
       <c r="C6">
-        <v>2.2999999999999998</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D6">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="6">
         <f>A3</f>
         <v>26</v>
       </c>
-      <c r="J6" s="19">
-        <f>C3</f>
-        <v>1.8</v>
-      </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19">
-        <f>C22</f>
-        <v>1.9</v>
-      </c>
-      <c r="M6" s="19">
-        <f>C24</f>
-        <v>3.9</v>
-      </c>
-      <c r="N6" s="19">
-        <f>C26</f>
-        <v>2.4</v>
-      </c>
-      <c r="O6" s="19">
-        <f>C28</f>
-        <v>2.5</v>
-      </c>
-      <c r="P6" s="19">
-        <f>C30</f>
-        <v>2.5</v>
-      </c>
-      <c r="Q6" s="19">
-        <f>C32</f>
-        <v>3.7</v>
-      </c>
-      <c r="R6" s="19">
-        <f>C34</f>
-        <v>5.5</v>
-      </c>
-      <c r="S6" s="19">
-        <f>C36</f>
-        <v>5.4</v>
-      </c>
-      <c r="T6" s="20">
-        <f>C38</f>
+      <c r="J6" s="11">
+        <f>$C3</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11">
+        <f>$C22</f>
+        <v>2.6</v>
+      </c>
+      <c r="M6" s="11">
+        <f>$C24</f>
+        <v>3.8</v>
+      </c>
+      <c r="N6" s="11">
+        <f>$C26</f>
+        <v>4.7</v>
+      </c>
+      <c r="O6" s="11">
+        <f>$C28</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P6" s="11">
+        <f>$C30</f>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="11">
+        <f>$C32</f>
+        <v>3</v>
+      </c>
+      <c r="R6" s="11">
+        <f>$C34</f>
         <v>4.9000000000000004</v>
+      </c>
+      <c r="S6" s="11">
+        <f>$C36</f>
+        <v>5.2</v>
+      </c>
+      <c r="T6" s="12">
+        <f>$C38</f>
+        <v>5.7</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1382,66 +1377,66 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="D7">
-        <v>3.4</v>
+        <v>1.9</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="6">
         <f>A5</f>
         <v>51</v>
       </c>
-      <c r="J7" s="19">
-        <f>C5</f>
-        <v>2.8</v>
-      </c>
-      <c r="K7" s="19">
-        <f>C23</f>
-        <v>1.6</v>
-      </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="19">
-        <f>C40</f>
-        <v>5</v>
-      </c>
-      <c r="N7" s="19">
-        <f>C42</f>
+      <c r="J7" s="11">
+        <f>$C5</f>
+        <v>1.8</v>
+      </c>
+      <c r="K7" s="11">
+        <f>$C23</f>
+        <v>1.7</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11">
+        <f>$C40</f>
+        <v>3.2</v>
+      </c>
+      <c r="N7" s="11">
+        <f>$C42</f>
+        <v>4</v>
+      </c>
+      <c r="O7" s="11">
+        <f>$C44</f>
+        <v>2.9</v>
+      </c>
+      <c r="P7" s="11">
+        <f>$C46</f>
         <v>4.3</v>
       </c>
-      <c r="O7" s="19">
-        <f>C44</f>
-        <v>2.6</v>
-      </c>
-      <c r="P7" s="19">
-        <f>C46</f>
-        <v>3.6</v>
-      </c>
-      <c r="Q7" s="19">
-        <f>C48</f>
+      <c r="Q7" s="11">
+        <f>$C48</f>
         <v>4.7</v>
       </c>
-      <c r="R7" s="19">
-        <f>C50</f>
-        <v>5.6</v>
-      </c>
-      <c r="S7" s="19">
-        <f>C52</f>
-        <v>5.8</v>
-      </c>
-      <c r="T7" s="20">
-        <f>C54</f>
-        <v>4.9000000000000004</v>
+      <c r="R7" s="11">
+        <f>$C50</f>
+        <v>4.2</v>
+      </c>
+      <c r="S7" s="11">
+        <f>$C52</f>
+        <v>4.8</v>
+      </c>
+      <c r="T7" s="12">
+        <f>$C54</f>
+        <v>5.7</v>
       </c>
       <c r="V7" t="s">
-        <v>8</v>
-      </c>
-      <c r="W7" s="23">
+        <v>6</v>
+      </c>
+      <c r="W7" s="15">
         <f>AVERAGE(J5:T15)</f>
-        <v>4.2936363636363621</v>
+        <v>4.743636363636365</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1452,66 +1447,66 @@
         <v>102</v>
       </c>
       <c r="C8">
-        <v>3.3</v>
+        <v>4.7</v>
       </c>
       <c r="D8">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="6">
         <f>A7</f>
         <v>77</v>
       </c>
-      <c r="J8" s="19">
-        <f>C7</f>
-        <v>3.4</v>
-      </c>
-      <c r="K8" s="19">
-        <f>C25</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L8" s="19">
-        <f>C41</f>
-        <v>1.9</v>
-      </c>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19">
-        <f>C56</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O8" s="19">
-        <f>C58</f>
-        <v>4.8</v>
-      </c>
-      <c r="P8" s="19">
-        <f>C60</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="Q8" s="19">
-        <f>C62</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="R8" s="19">
-        <f>C64</f>
+      <c r="J8" s="11">
+        <f>$C7</f>
+        <v>2.4</v>
+      </c>
+      <c r="K8" s="11">
+        <f>$C25</f>
+        <v>2.1</v>
+      </c>
+      <c r="L8" s="11">
+        <f>$C41</f>
+        <v>4.7</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11">
+        <f>$C56</f>
+        <v>2.7</v>
+      </c>
+      <c r="O8" s="11">
+        <f>$C58</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P8" s="11">
+        <f>$C60</f>
+        <v>2.8</v>
+      </c>
+      <c r="Q8" s="11">
+        <f>$C62</f>
+        <v>4.7</v>
+      </c>
+      <c r="R8" s="11">
+        <f>$C64</f>
+        <v>3.7</v>
+      </c>
+      <c r="S8" s="11">
+        <f>$C66</f>
+        <v>5.4</v>
+      </c>
+      <c r="T8" s="12">
+        <f>$C68</f>
         <v>5.6</v>
       </c>
-      <c r="S8" s="19">
-        <f>C66</f>
-        <v>5.6</v>
-      </c>
-      <c r="T8" s="20">
-        <f>C68</f>
-        <v>4.8</v>
-      </c>
       <c r="V8" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="23">
+        <v>7</v>
+      </c>
+      <c r="W8" s="15">
         <f>AVERAGE(K5,L5:L6,M5:M7,N5:N8,O5:O9,P5:P10,Q5:Q11,R5:R12,S5:S13,T5:T14)</f>
-        <v>4.5509090909090908</v>
+        <v>4.3018181818181809</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1522,66 +1517,66 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="D9">
-        <v>3.9</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="6">
         <f>A9</f>
         <v>102</v>
       </c>
-      <c r="J9" s="19">
-        <f>C9</f>
-        <v>3.9</v>
-      </c>
-      <c r="K9" s="19">
-        <f>C27</f>
-        <v>2.4</v>
-      </c>
-      <c r="L9" s="19">
-        <f>C43</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M9" s="19">
-        <f>C57</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="19">
-        <f>C70</f>
-        <v>5.3</v>
-      </c>
-      <c r="P9" s="19">
-        <f>C72</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="Q9" s="19">
-        <f>C74</f>
-        <v>5.3</v>
-      </c>
-      <c r="R9" s="19">
-        <f>C76</f>
+      <c r="J9" s="11">
+        <f>$C9</f>
+        <v>2.9</v>
+      </c>
+      <c r="K9" s="11">
+        <f>$C27</f>
+        <v>2.6</v>
+      </c>
+      <c r="L9" s="11">
+        <f>$C43</f>
+        <v>5.2</v>
+      </c>
+      <c r="M9" s="11">
+        <f>$C57</f>
+        <v>4.8</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="11">
+        <f>$C70</f>
+        <v>4.5</v>
+      </c>
+      <c r="P9" s="11">
+        <f>$C72</f>
+        <v>5.4</v>
+      </c>
+      <c r="Q9" s="11">
+        <f>$C74</f>
         <v>5.6</v>
       </c>
-      <c r="S9" s="19">
-        <f>C78</f>
+      <c r="R9" s="11">
+        <f>$C76</f>
+        <v>4.3</v>
+      </c>
+      <c r="S9" s="11">
+        <f>$C78</f>
+        <v>4.2</v>
+      </c>
+      <c r="T9" s="12">
+        <f>$C80</f>
         <v>5.7</v>
       </c>
-      <c r="T9" s="20">
-        <f>C80</f>
-        <v>4.8</v>
-      </c>
       <c r="V9" t="s">
-        <v>10</v>
-      </c>
-      <c r="W9" s="23">
+        <v>8</v>
+      </c>
+      <c r="W9" s="15">
         <f>AVERAGE(J6:J15,K7:K15,L8:L15,M9:M15,N10:N15,O11:O15,P12:P15,Q13:Q15,R14:R15,S15)</f>
-        <v>4.0363636363636379</v>
+        <v>5.1854545454545464</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1592,66 +1587,66 @@
         <v>128</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>2.9</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="6">
         <f>A11</f>
         <v>128</v>
       </c>
-      <c r="J10" s="19">
-        <f>C11</f>
-        <v>4.3</v>
-      </c>
-      <c r="K10" s="19">
-        <f>C29</f>
-        <v>2.7</v>
-      </c>
-      <c r="L10" s="19">
-        <f>C45</f>
-        <v>2.4</v>
-      </c>
-      <c r="M10" s="19">
-        <f>C59</f>
-        <v>2.5</v>
-      </c>
-      <c r="N10" s="19">
-        <f>C71</f>
-        <v>4</v>
-      </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="19">
-        <f>C82</f>
-        <v>5.2</v>
-      </c>
-      <c r="Q10" s="19">
-        <f>C84</f>
-        <v>5.4</v>
-      </c>
-      <c r="R10" s="19">
-        <f>C86</f>
-        <v>5.7</v>
-      </c>
-      <c r="S10" s="19">
-        <f>C88</f>
-        <v>5.6</v>
-      </c>
-      <c r="T10" s="20">
-        <f>C90</f>
-        <v>4.5999999999999996</v>
+      <c r="J10" s="11">
+        <f>$C11</f>
+        <v>3.4</v>
+      </c>
+      <c r="K10" s="11">
+        <f>$C29</f>
+        <v>2.9</v>
+      </c>
+      <c r="L10" s="11">
+        <f>$C45</f>
+        <v>5.3</v>
+      </c>
+      <c r="M10" s="11">
+        <f>$C59</f>
+        <v>5.8</v>
+      </c>
+      <c r="N10" s="11">
+        <f>$C71</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="11">
+        <f>$C82</f>
+        <v>5.3</v>
+      </c>
+      <c r="Q10" s="11">
+        <f>$C84</f>
+        <v>5.8</v>
+      </c>
+      <c r="R10" s="11">
+        <f>$C86</f>
+        <v>3.6</v>
+      </c>
+      <c r="S10" s="11">
+        <f>$C88</f>
+        <v>3.5</v>
+      </c>
+      <c r="T10" s="12">
+        <f>$C90</f>
+        <v>5.0999999999999996</v>
       </c>
       <c r="V10" t="s">
-        <v>11</v>
-      </c>
-      <c r="W10" s="24">
+        <v>9</v>
+      </c>
+      <c r="W10" s="16">
         <f>T5+J15</f>
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1662,66 +1657,66 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>4.3</v>
+        <v>3.4</v>
       </c>
       <c r="D11">
-        <v>4.3</v>
+        <v>2.1</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="6">
         <f>A13</f>
         <v>153</v>
       </c>
-      <c r="J11" s="19">
-        <f>C13</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K11" s="19">
-        <f>C31</f>
+      <c r="J11" s="11">
+        <f>$C13</f>
         <v>3.5</v>
       </c>
-      <c r="L11" s="19">
-        <f>C47</f>
+      <c r="K11" s="11">
+        <f>$C31</f>
+        <v>3.8</v>
+      </c>
+      <c r="L11" s="11">
+        <f>$C47</f>
+        <v>5</v>
+      </c>
+      <c r="M11" s="11">
+        <f>$C61</f>
+        <v>7</v>
+      </c>
+      <c r="N11" s="11">
+        <f>$C73</f>
+        <v>7</v>
+      </c>
+      <c r="O11" s="11">
+        <f>$C83</f>
+        <v>5.2</v>
+      </c>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11">
+        <f>$C92</f>
+        <v>2.6</v>
+      </c>
+      <c r="R11" s="11">
+        <f>$C94</f>
         <v>2.8</v>
       </c>
-      <c r="M11" s="19">
-        <f>C61</f>
-        <v>2.8</v>
-      </c>
-      <c r="N11" s="19">
-        <f>C73</f>
-        <v>2.5</v>
-      </c>
-      <c r="O11" s="19">
-        <f>C83</f>
-        <v>4.3</v>
-      </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19">
-        <f>C92</f>
-        <v>5.4</v>
-      </c>
-      <c r="R11" s="19">
-        <f>C94</f>
-        <v>5.5</v>
-      </c>
-      <c r="S11" s="19">
-        <f>C96</f>
-        <v>5.6</v>
-      </c>
-      <c r="T11" s="20">
-        <f>C98</f>
+      <c r="S11" s="11">
+        <f>$C96</f>
         <v>4.5</v>
       </c>
+      <c r="T11" s="12">
+        <f>$C98</f>
+        <v>4.7</v>
+      </c>
       <c r="V11" t="s">
-        <v>12</v>
-      </c>
-      <c r="W11" s="24">
+        <v>10</v>
+      </c>
+      <c r="W11" s="16">
         <f>MIN(J5:T15)</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1732,66 +1727,66 @@
         <v>153</v>
       </c>
       <c r="C12">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="D12">
-        <v>3.5</v>
+        <v>2.6</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="6">
         <f>A15</f>
         <v>179</v>
       </c>
-      <c r="J12" s="19">
-        <f>C15</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="K12" s="19">
-        <f>C33</f>
+      <c r="J12" s="11">
+        <f>$C15</f>
+        <v>3.8</v>
+      </c>
+      <c r="K12" s="11">
+        <f>$C33</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="L12" s="19">
-        <f>C49</f>
-        <v>2.8</v>
-      </c>
-      <c r="M12" s="19">
-        <f>C63</f>
-        <v>3.7</v>
-      </c>
-      <c r="N12" s="19">
-        <f>C75</f>
-        <v>2.9</v>
-      </c>
-      <c r="O12" s="19">
-        <f>C85</f>
-        <v>2.5</v>
-      </c>
-      <c r="P12" s="19">
-        <f>C93</f>
-        <v>4.3</v>
-      </c>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="19">
-        <f>C100</f>
-        <v>5.4</v>
-      </c>
-      <c r="S12" s="19">
-        <f>C102</f>
-        <v>5.6</v>
-      </c>
-      <c r="T12" s="20">
-        <f>C104</f>
+      <c r="L12" s="11">
+        <f>$C49</f>
         <v>4.5</v>
       </c>
+      <c r="M12" s="11">
+        <f>$C63</f>
+        <v>6.7</v>
+      </c>
+      <c r="N12" s="11">
+        <f>$C75</f>
+        <v>7.4</v>
+      </c>
+      <c r="O12" s="11">
+        <f>$C85</f>
+        <v>7.2</v>
+      </c>
+      <c r="P12" s="11">
+        <f>$C93</f>
+        <v>5.2</v>
+      </c>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="11">
+        <f>$C100</f>
+        <v>2.6</v>
+      </c>
+      <c r="S12" s="11">
+        <f>$C102</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="T12" s="12">
+        <f>$C104</f>
+        <v>4.5</v>
+      </c>
       <c r="V12" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="24">
+        <v>11</v>
+      </c>
+      <c r="W12" s="16">
         <f>MAX(J5:T15)</f>
-        <v>7</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1802,59 +1797,59 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>4.5999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="D13">
-        <v>4.5999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="6">
         <f>A17</f>
         <v>204</v>
       </c>
-      <c r="J13" s="19">
-        <f>C17</f>
-        <v>5.3</v>
-      </c>
-      <c r="K13" s="19">
-        <f>C35</f>
-        <v>5.4</v>
-      </c>
-      <c r="L13" s="19">
-        <f>C51</f>
-        <v>2.7</v>
-      </c>
-      <c r="M13" s="19">
-        <f>C65</f>
-        <v>3.9</v>
-      </c>
-      <c r="N13" s="19">
-        <f>C77</f>
+      <c r="J13" s="11">
+        <f>$C17</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K13" s="11">
+        <f>$C35</f>
+        <v>5</v>
+      </c>
+      <c r="L13" s="11">
+        <f>$C51</f>
+        <v>3.1</v>
+      </c>
+      <c r="M13" s="11">
+        <f>$C65</f>
+        <v>6.3</v>
+      </c>
+      <c r="N13" s="11">
+        <f>$C77</f>
+        <v>7.6</v>
+      </c>
+      <c r="O13" s="11">
+        <f>$C87</f>
+        <v>7.7</v>
+      </c>
+      <c r="P13" s="11">
+        <f>$C95</f>
+        <v>7.1</v>
+      </c>
+      <c r="Q13" s="11">
+        <f>$C101</f>
+        <v>6.4</v>
+      </c>
+      <c r="R13" s="10"/>
+      <c r="S13" s="11">
+        <f>$C106</f>
         <v>4.8</v>
       </c>
-      <c r="O13" s="19">
-        <f>C87</f>
-        <v>2.7</v>
-      </c>
-      <c r="P13" s="19">
-        <f>C95</f>
-        <v>4.2</v>
-      </c>
-      <c r="Q13" s="19">
-        <f>C101</f>
-        <v>4.3</v>
-      </c>
-      <c r="R13" s="18"/>
-      <c r="S13" s="19">
-        <f>C106</f>
-        <v>5.6</v>
-      </c>
-      <c r="T13" s="20">
-        <f>C108</f>
-        <v>3.9</v>
+      <c r="T13" s="12">
+        <f>$C108</f>
+        <v>3.3</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1865,59 +1860,59 @@
         <v>179</v>
       </c>
       <c r="C14">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="D14">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="19"/>
       <c r="I14" s="6">
         <f>A19</f>
         <v>230</v>
       </c>
-      <c r="J14" s="19">
-        <f>C19</f>
+      <c r="J14" s="11">
+        <f>$C19</f>
+        <v>4.3</v>
+      </c>
+      <c r="K14" s="11">
+        <f>$C37</f>
+        <v>5.3</v>
+      </c>
+      <c r="L14" s="11">
+        <f>$C53</f>
+        <v>4.2</v>
+      </c>
+      <c r="M14" s="11">
+        <f>$C67</f>
         <v>5.4</v>
       </c>
-      <c r="K14" s="19">
-        <f>C37</f>
-        <v>6</v>
-      </c>
-      <c r="L14" s="19">
-        <f>C53</f>
-        <v>3.5</v>
-      </c>
-      <c r="M14" s="19">
-        <f>C67</f>
-        <v>4.7</v>
-      </c>
-      <c r="N14" s="19">
-        <f>C79</f>
-        <v>5.5</v>
-      </c>
-      <c r="O14" s="19">
-        <f>C89</f>
-        <v>3.9</v>
-      </c>
-      <c r="P14" s="19">
-        <f>C97</f>
-        <v>3</v>
-      </c>
-      <c r="Q14" s="19">
-        <f>C103</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="R14" s="19">
-        <f>C107</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="S14" s="18"/>
-      <c r="T14" s="20">
+      <c r="N14" s="11">
+        <f>$C79</f>
+        <v>7.3</v>
+      </c>
+      <c r="O14" s="11">
+        <f>$C89</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="P14" s="11">
+        <f>$C97</f>
+        <v>7.8</v>
+      </c>
+      <c r="Q14" s="11">
+        <f>$C103</f>
+        <v>7.1</v>
+      </c>
+      <c r="R14" s="11">
+        <f>$C107</f>
+        <v>6.3</v>
+      </c>
+      <c r="S14" s="10"/>
+      <c r="T14" s="12">
         <f>C110</f>
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1928,60 +1923,60 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>4.9000000000000004</v>
+        <v>3.8</v>
       </c>
       <c r="D15">
-        <v>4.9000000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="7">
         <f>A21</f>
         <v>255</v>
       </c>
-      <c r="J15" s="21">
-        <f>C21</f>
+      <c r="J15" s="13">
+        <f>$C21</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K15" s="13">
+        <f>$C39</f>
         <v>5.7</v>
       </c>
-      <c r="K15" s="21">
-        <f>C39</f>
+      <c r="L15" s="13">
+        <f>$C55</f>
+        <v>5.4</v>
+      </c>
+      <c r="M15" s="13">
+        <f>$C69</f>
+        <v>3.7</v>
+      </c>
+      <c r="N15" s="13">
+        <f>$C81</f>
         <v>6.5</v>
       </c>
-      <c r="L15" s="21">
-        <f>C55</f>
-        <v>5.9</v>
-      </c>
-      <c r="M15" s="21">
-        <f>C69</f>
-        <v>6.6</v>
-      </c>
-      <c r="N15" s="21">
-        <f>C81</f>
-        <v>5.9</v>
-      </c>
-      <c r="O15" s="21">
-        <f>C91</f>
-        <v>2.8</v>
-      </c>
-      <c r="P15" s="21">
-        <f>C99</f>
+      <c r="O15" s="13">
+        <f>$C91</f>
+        <v>7.6</v>
+      </c>
+      <c r="P15" s="13">
+        <f>$C99</f>
+        <v>7.8</v>
+      </c>
+      <c r="Q15" s="13">
+        <f>$C105</f>
+        <v>7.3</v>
+      </c>
+      <c r="R15" s="13">
+        <f>$C109</f>
         <v>6.3</v>
       </c>
-      <c r="Q15" s="21">
-        <f>C105</f>
-        <v>6.7</v>
-      </c>
-      <c r="R15" s="21">
-        <f>C109</f>
-        <v>7</v>
-      </c>
-      <c r="S15" s="21">
-        <f>C111</f>
-        <v>6.4</v>
-      </c>
-      <c r="T15" s="22"/>
+      <c r="S15" s="13">
+        <f>$C111</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="T15" s="14"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1991,13 +1986,13 @@
         <v>204</v>
       </c>
       <c r="C16">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="D16">
-        <v>5.0999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -2008,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>5.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D17">
-        <v>5.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2025,21 +2020,21 @@
         <v>230</v>
       </c>
       <c r="C18">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="D18">
-        <v>5.7</v>
+        <v>2.8</v>
       </c>
       <c r="E18">
-        <v>1.3</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -2049,10 +2044,10 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>5.4</v>
+        <v>4.3</v>
       </c>
       <c r="D19">
-        <v>5.4</v>
+        <v>2.4</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2066,33 +2061,34 @@
         <v>255</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>5.9</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>2.8</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="23"/>
+      <c r="V20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="12"/>
-      <c r="V20" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="W20" s="9">
+        <f>W3</f>
         <v>165</v>
       </c>
     </row>
@@ -2104,10 +2100,10 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>5.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D21">
-        <v>5.7</v>
+        <v>2.4</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -2159,7 +2155,7 @@
         <v>255</v>
       </c>
       <c r="V21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W21" s="8">
         <f>1000/W20</f>
@@ -2174,68 +2170,68 @@
         <v>51</v>
       </c>
       <c r="C22">
-        <v>1.9</v>
+        <v>2.6</v>
       </c>
       <c r="D22">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>4</v>
+      <c r="H22" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="I22" s="5">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19">
+      <c r="J22" s="10"/>
+      <c r="K22" s="11">
         <f>D2</f>
-        <v>1.7</v>
-      </c>
-      <c r="L22" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="L22" s="11">
         <f>D4</f>
-        <v>3.7</v>
-      </c>
-      <c r="M22" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="M22" s="11">
         <f>D6</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N22" s="19">
+        <v>2.7</v>
+      </c>
+      <c r="N22" s="11">
         <f>D8</f>
-        <v>3.3</v>
-      </c>
-      <c r="O22" s="19">
+        <v>2.8</v>
+      </c>
+      <c r="O22" s="11">
         <f>D10</f>
+        <v>2.9</v>
+      </c>
+      <c r="P22" s="11">
+        <f>D12</f>
+        <v>2.6</v>
+      </c>
+      <c r="Q22" s="11">
+        <f>D14</f>
+        <v>2.4</v>
+      </c>
+      <c r="R22" s="11">
+        <f>D16</f>
+        <v>2.5</v>
+      </c>
+      <c r="S22" s="11">
+        <f>D18</f>
+        <v>2.8</v>
+      </c>
+      <c r="T22" s="12">
+        <f>D20</f>
+        <v>2.8</v>
+      </c>
+      <c r="V22" t="s">
         <v>5</v>
-      </c>
-      <c r="P22" s="19">
-        <f>D12</f>
-        <v>3.5</v>
-      </c>
-      <c r="Q22" s="19">
-        <f>D14</f>
-        <v>2.5</v>
-      </c>
-      <c r="R22" s="19">
-        <f>D16</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="S22" s="19">
-        <f>D18</f>
-        <v>5.7</v>
-      </c>
-      <c r="T22" s="20">
-        <f>D20</f>
-        <v>5</v>
-      </c>
-      <c r="V22" t="s">
-        <v>7</v>
       </c>
       <c r="W22" s="8">
         <f>((COUNTIF(J22:T32, "&lt;" &amp;W21))/110)*100</f>
-        <v>94.545454545454547</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2246,59 +2242,59 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="D23">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="6">
         <f>A3</f>
         <v>26</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="11">
         <f>D3</f>
-        <v>1.8</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11">
         <f>D22</f>
-        <v>1.9</v>
-      </c>
-      <c r="M23" s="19">
+        <v>2</v>
+      </c>
+      <c r="M23" s="11">
         <f>D24</f>
-        <v>3.9</v>
-      </c>
-      <c r="N23" s="19">
+        <v>2.7</v>
+      </c>
+      <c r="N23" s="11">
         <f>D26</f>
-        <v>2.4</v>
-      </c>
-      <c r="O23" s="19">
+        <v>2.9</v>
+      </c>
+      <c r="O23" s="11">
         <f>D28</f>
+        <v>2.7</v>
+      </c>
+      <c r="P23" s="11">
+        <f>D30</f>
+        <v>2.7</v>
+      </c>
+      <c r="Q23" s="11">
+        <f>D32</f>
         <v>2.5</v>
       </c>
-      <c r="P23" s="19">
-        <f>D30</f>
-        <v>2.5</v>
-      </c>
-      <c r="Q23" s="19">
-        <f>D32</f>
-        <v>3.7</v>
-      </c>
-      <c r="R23" s="19">
+      <c r="R23" s="11">
         <f>D34</f>
-        <v>5.5</v>
-      </c>
-      <c r="S23" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="S23" s="11">
         <f>D36</f>
-        <v>5.4</v>
-      </c>
-      <c r="T23" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="T23" s="12">
         <f>D38</f>
-        <v>4.9000000000000004</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -2309,66 +2305,66 @@
         <v>77</v>
       </c>
       <c r="C24">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="D24">
-        <v>3.9</v>
+        <v>2.7</v>
       </c>
       <c r="E24">
-        <v>1.3</v>
-      </c>
-      <c r="H24" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="19"/>
       <c r="I24" s="6">
         <f>A5</f>
         <v>51</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="11">
         <f>D5</f>
-        <v>2.8</v>
-      </c>
-      <c r="K24" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="K24" s="11">
         <f>D23</f>
-        <v>1.6</v>
-      </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11">
         <f>D40</f>
-        <v>5</v>
-      </c>
-      <c r="N24" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N24" s="11">
         <f>D42</f>
-        <v>4.3</v>
-      </c>
-      <c r="O24" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="O24" s="11">
         <f>D44</f>
+        <v>2.5</v>
+      </c>
+      <c r="P24" s="11">
+        <f>D46</f>
         <v>2.6</v>
       </c>
-      <c r="P24" s="19">
-        <f>D46</f>
-        <v>3.6</v>
-      </c>
-      <c r="Q24" s="19">
+      <c r="Q24" s="11">
         <f>D48</f>
-        <v>4.7</v>
-      </c>
-      <c r="R24" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="R24" s="11">
         <f>D50</f>
-        <v>5.6</v>
-      </c>
-      <c r="S24" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="S24" s="11">
         <f>D52</f>
-        <v>5.8</v>
-      </c>
-      <c r="T24" s="20">
+        <v>2.6</v>
+      </c>
+      <c r="T24" s="12">
         <f>D54</f>
-        <v>4.9000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="V24" t="s">
-        <v>24</v>
-      </c>
-      <c r="W24" s="23">
+        <v>21</v>
+      </c>
+      <c r="W24" s="15">
         <f>W7</f>
-        <v>4.2936363636363621</v>
+        <v>4.743636363636365</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -2379,66 +2375,66 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="D25">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="H25" s="14"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="6">
         <f>A7</f>
         <v>77</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="11">
         <f>D7</f>
-        <v>3.4</v>
-      </c>
-      <c r="K25" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="K25" s="11">
         <f>D25</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L25" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="L25" s="11">
         <f>D41</f>
-        <v>1.9</v>
-      </c>
-      <c r="M25" s="18"/>
-      <c r="N25" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="M25" s="10"/>
+      <c r="N25" s="11">
         <f>D56</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O25" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="O25" s="11">
         <f>D58</f>
-        <v>4.8</v>
-      </c>
-      <c r="P25" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P25" s="11">
         <f>D60</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="Q25" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="Q25" s="11">
         <f>D62</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="R25" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="R25" s="11">
         <f>D64</f>
-        <v>5.6</v>
-      </c>
-      <c r="S25" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="S25" s="11">
         <f>D66</f>
-        <v>5.6</v>
-      </c>
-      <c r="T25" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="T25" s="12">
         <f>D68</f>
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
       <c r="V25" t="s">
-        <v>8</v>
-      </c>
-      <c r="W25" s="23">
+        <v>6</v>
+      </c>
+      <c r="W25" s="15">
         <f>AVERAGE(J22:T32)</f>
-        <v>4.2936363636363621</v>
+        <v>2.1772727272727268</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -2449,66 +2445,66 @@
         <v>102</v>
       </c>
       <c r="C26">
-        <v>2.4</v>
+        <v>4.7</v>
       </c>
       <c r="D26">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="H26" s="14"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="6">
         <f>A9</f>
         <v>102</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="11">
         <f>D9</f>
-        <v>3.9</v>
-      </c>
-      <c r="K26" s="19">
+        <v>2</v>
+      </c>
+      <c r="K26" s="11">
         <f>D27</f>
-        <v>2.4</v>
-      </c>
-      <c r="L26" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="L26" s="11">
         <f>D43</f>
+        <v>1.5</v>
+      </c>
+      <c r="M26" s="11">
+        <f>D57</f>
+        <v>1.6</v>
+      </c>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11">
+        <f>D70</f>
+        <v>2.1</v>
+      </c>
+      <c r="P26" s="11">
+        <f>D72</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="M26" s="19">
-        <f>D57</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19">
-        <f>D70</f>
-        <v>5.3</v>
-      </c>
-      <c r="P26" s="19">
-        <f>D72</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="Q26" s="19">
+      <c r="Q26" s="11">
         <f>D74</f>
-        <v>5.3</v>
-      </c>
-      <c r="R26" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R26" s="11">
         <f>D76</f>
-        <v>5.6</v>
-      </c>
-      <c r="S26" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="S26" s="11">
         <f>D78</f>
-        <v>5.7</v>
-      </c>
-      <c r="T26" s="20">
+        <v>2.6</v>
+      </c>
+      <c r="T26" s="12">
         <f>D80</f>
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
       <c r="V26" t="s">
-        <v>9</v>
-      </c>
-      <c r="W26" s="23">
+        <v>7</v>
+      </c>
+      <c r="W26" s="15">
         <f>AVERAGE(K22,L22:L23,M22:M24,N22:N25,O22:O26,P22:P27,Q22:Q28,R22:R29,S22:S30,T22:T31)</f>
-        <v>4.5509090909090908</v>
+        <v>2.4254545454545449</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -2519,66 +2515,66 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="D27">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="H27" s="14"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="6">
         <f>A11</f>
         <v>128</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="11">
         <f>D11</f>
-        <v>4.3</v>
-      </c>
-      <c r="K27" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="K27" s="11">
         <f>D29</f>
-        <v>2.7</v>
-      </c>
-      <c r="L27" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L27" s="11">
         <f>D45</f>
+        <v>1.8</v>
+      </c>
+      <c r="M27" s="11">
+        <f>D59</f>
+        <v>1.6</v>
+      </c>
+      <c r="N27" s="11">
+        <f>D71</f>
+        <v>1.9</v>
+      </c>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11">
+        <f>D82</f>
+        <v>2</v>
+      </c>
+      <c r="Q27" s="11">
+        <f>D84</f>
+        <v>2</v>
+      </c>
+      <c r="R27" s="11">
+        <f>D86</f>
         <v>2.4</v>
       </c>
-      <c r="M27" s="19">
-        <f>D59</f>
+      <c r="S27" s="11">
+        <f>D88</f>
         <v>2.5</v>
       </c>
-      <c r="N27" s="19">
-        <f>D71</f>
-        <v>4</v>
-      </c>
-      <c r="O27" s="18"/>
-      <c r="P27" s="19">
-        <f>D82</f>
-        <v>5.2</v>
-      </c>
-      <c r="Q27" s="19">
-        <f>D84</f>
-        <v>5.4</v>
-      </c>
-      <c r="R27" s="19">
-        <f>D86</f>
-        <v>5.7</v>
-      </c>
-      <c r="S27" s="19">
-        <f>D88</f>
-        <v>5.6</v>
-      </c>
-      <c r="T27" s="20">
+      <c r="T27" s="12">
         <f>D90</f>
-        <v>4.5999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="V27" t="s">
-        <v>10</v>
-      </c>
-      <c r="W27" s="23">
+        <v>8</v>
+      </c>
+      <c r="W27" s="15">
         <f>AVERAGE(J23:J32,K24:K32,L25:L32,M26:M32,N27:N32,O28:O32,P29:P32,Q30:Q32,R31:R32,S32)</f>
-        <v>4.0363636363636379</v>
+        <v>1.9290909090909099</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -2589,66 +2585,66 @@
         <v>128</v>
       </c>
       <c r="C28">
-        <v>2.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D28">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="H28" s="14"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="6">
         <f>A13</f>
         <v>153</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="11">
         <f>D13</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K28" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K28" s="11">
         <f>D31</f>
-        <v>3.5</v>
-      </c>
-      <c r="L28" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L28" s="11">
         <f>D47</f>
-        <v>2.8</v>
-      </c>
-      <c r="M28" s="19">
+        <v>2</v>
+      </c>
+      <c r="M28" s="11">
         <f>D61</f>
-        <v>2.8</v>
-      </c>
-      <c r="N28" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="N28" s="11">
         <f>D73</f>
-        <v>2.5</v>
-      </c>
-      <c r="O28" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="O28" s="11">
         <f>D83</f>
-        <v>4.3</v>
-      </c>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="11">
         <f>D92</f>
-        <v>5.4</v>
-      </c>
-      <c r="R28" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R28" s="11">
         <f>D94</f>
-        <v>5.5</v>
-      </c>
-      <c r="S28" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S28" s="11">
         <f>D96</f>
-        <v>5.6</v>
-      </c>
-      <c r="T28" s="20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T28" s="12">
         <f>D98</f>
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="V28" t="s">
-        <v>11</v>
-      </c>
-      <c r="W28" s="24">
+        <v>9</v>
+      </c>
+      <c r="W28" s="16">
         <f>T22+J32</f>
-        <v>10.7</v>
+        <v>5.1999999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -2659,66 +2655,66 @@
         <v>26</v>
       </c>
       <c r="C29">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="D29">
-        <v>2.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="6">
         <f>A15</f>
         <v>179</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="11">
         <f>D15</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="K29" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K29" s="11">
         <f>D33</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L29" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="L29" s="11">
         <f>D49</f>
-        <v>2.8</v>
-      </c>
-      <c r="M29" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M29" s="11">
         <f>D63</f>
-        <v>3.7</v>
-      </c>
-      <c r="N29" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="N29" s="11">
         <f>D75</f>
-        <v>2.9</v>
-      </c>
-      <c r="O29" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="O29" s="11">
         <f>D85</f>
-        <v>2.5</v>
-      </c>
-      <c r="P29" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="P29" s="11">
         <f>D93</f>
-        <v>4.3</v>
-      </c>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="11">
         <f>D100</f>
-        <v>5.4</v>
-      </c>
-      <c r="S29" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="S29" s="11">
         <f>D102</f>
-        <v>5.6</v>
-      </c>
-      <c r="T29" s="20">
+        <v>2</v>
+      </c>
+      <c r="T29" s="12">
         <f>D104</f>
-        <v>4.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="V29" t="s">
-        <v>12</v>
-      </c>
-      <c r="W29" s="24">
+        <v>10</v>
+      </c>
+      <c r="W29" s="16">
         <f>MIN(J22:T32)</f>
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -2729,66 +2725,66 @@
         <v>153</v>
       </c>
       <c r="C30">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="D30">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="H30" s="14"/>
+      <c r="H30" s="19"/>
       <c r="I30" s="6">
         <f>A17</f>
         <v>204</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="11">
         <f>D17</f>
-        <v>5.3</v>
-      </c>
-      <c r="K30" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K30" s="11">
         <f>D35</f>
-        <v>5.4</v>
-      </c>
-      <c r="L30" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="L30" s="11">
         <f>D51</f>
-        <v>2.7</v>
-      </c>
-      <c r="M30" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M30" s="11">
         <f>D65</f>
-        <v>3.9</v>
-      </c>
-      <c r="N30" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="N30" s="11">
         <f>D77</f>
-        <v>4.8</v>
-      </c>
-      <c r="O30" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="O30" s="11">
         <f>D87</f>
-        <v>2.7</v>
-      </c>
-      <c r="P30" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="P30" s="11">
         <f>D95</f>
-        <v>4.2</v>
-      </c>
-      <c r="Q30" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="Q30" s="11">
         <f>D101</f>
-        <v>4.3</v>
-      </c>
-      <c r="R30" s="18"/>
-      <c r="S30" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="R30" s="10"/>
+      <c r="S30" s="11">
         <f>D106</f>
-        <v>5.6</v>
-      </c>
-      <c r="T30" s="20">
+        <v>2</v>
+      </c>
+      <c r="T30" s="12">
         <f>D108</f>
-        <v>3.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="V30" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" s="24">
+        <v>11</v>
+      </c>
+      <c r="W30" s="16">
         <f>MAX(J22:T32)</f>
-        <v>7</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -2799,59 +2795,59 @@
         <v>26</v>
       </c>
       <c r="C31">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="D31">
-        <v>3.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="H31" s="14"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="6">
         <f>A19</f>
         <v>230</v>
       </c>
-      <c r="J31" s="19">
+      <c r="J31" s="11">
         <f>D19</f>
-        <v>5.4</v>
-      </c>
-      <c r="K31" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="K31" s="11">
         <f>D37</f>
-        <v>6</v>
-      </c>
-      <c r="L31" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="L31" s="11">
         <f>D53</f>
-        <v>3.5</v>
-      </c>
-      <c r="M31" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="M31" s="11">
         <f>D67</f>
-        <v>4.7</v>
-      </c>
-      <c r="N31" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N31" s="11">
         <f>D79</f>
-        <v>5.5</v>
-      </c>
-      <c r="O31" s="19">
+        <v>2</v>
+      </c>
+      <c r="O31" s="11">
         <f>D89</f>
-        <v>3.9</v>
-      </c>
-      <c r="P31" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="P31" s="11">
         <f>D97</f>
-        <v>3</v>
-      </c>
-      <c r="Q31" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="Q31" s="11">
         <f>D103</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="R31" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="R31" s="11">
         <f>D107</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="S31" s="18"/>
-      <c r="T31" s="20">
+        <v>1.7</v>
+      </c>
+      <c r="S31" s="10"/>
+      <c r="T31" s="12">
         <f>D110</f>
-        <v>3.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2862,60 +2858,60 @@
         <v>179</v>
       </c>
       <c r="C32">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>3.7</v>
+        <v>2.5</v>
       </c>
       <c r="E32">
-        <v>0.6</v>
-      </c>
-      <c r="H32" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="20"/>
       <c r="I32" s="7">
         <f>A21</f>
         <v>255</v>
       </c>
-      <c r="J32" s="21">
+      <c r="J32" s="13">
         <f>D21</f>
-        <v>5.7</v>
-      </c>
-      <c r="K32" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="K32" s="13">
         <f>D39</f>
-        <v>6.5</v>
-      </c>
-      <c r="L32" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="L32" s="13">
         <f>D55</f>
-        <v>5.9</v>
-      </c>
-      <c r="M32" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="M32" s="13">
         <f>D69</f>
-        <v>6.6</v>
-      </c>
-      <c r="N32" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="N32" s="13">
         <f>D81</f>
-        <v>5.9</v>
-      </c>
-      <c r="O32" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O32" s="13">
         <f>D91</f>
-        <v>2.8</v>
-      </c>
-      <c r="P32" s="21">
+        <v>1.9</v>
+      </c>
+      <c r="P32" s="13">
         <f>D99</f>
-        <v>6.3</v>
-      </c>
-      <c r="Q32" s="21">
+        <v>1.7</v>
+      </c>
+      <c r="Q32" s="13">
         <f>D105</f>
-        <v>6.7</v>
-      </c>
-      <c r="R32" s="21">
+        <v>1.7</v>
+      </c>
+      <c r="R32" s="13">
         <f>D109</f>
-        <v>7</v>
-      </c>
-      <c r="S32" s="21">
+        <v>1.9</v>
+      </c>
+      <c r="S32" s="13">
         <f>D111</f>
-        <v>6.4</v>
-      </c>
-      <c r="T32" s="22"/>
+        <v>1.9</v>
+      </c>
+      <c r="T32" s="14"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -2928,7 +2924,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D33">
-        <v>4.4000000000000004</v>
+        <v>2.4</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2942,21 +2938,21 @@
         <v>204</v>
       </c>
       <c r="C34">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D34">
-        <v>5.5</v>
+        <v>2.6</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
     </row>
     <row r="35" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -2966,10 +2962,10 @@
         <v>26</v>
       </c>
       <c r="C35">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="D35">
-        <v>5.4</v>
+        <v>2.4</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2983,34 +2979,34 @@
         <v>230</v>
       </c>
       <c r="C36">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
       <c r="D36">
-        <v>5.4</v>
+        <v>2.7</v>
       </c>
       <c r="E36">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="12"/>
+      <c r="J36" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="23"/>
       <c r="V36" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W36" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3021,10 +3017,10 @@
         <v>26</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>5.3</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>2.4</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -3084,68 +3080,68 @@
         <v>255</v>
       </c>
       <c r="C38">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
       <c r="D38">
-        <v>4.9000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>4</v>
+      <c r="H38" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="I38" s="5">
         <f>A2</f>
         <v>0</v>
       </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="19">
+      <c r="J38" s="10"/>
+      <c r="K38" s="11">
         <f>E2</f>
         <v>0</v>
       </c>
-      <c r="L38" s="19">
+      <c r="L38" s="11">
         <f>E4</f>
-        <v>3.9</v>
-      </c>
-      <c r="M38" s="19">
+        <v>0</v>
+      </c>
+      <c r="M38" s="11">
         <f>E6</f>
         <v>0</v>
       </c>
-      <c r="N38" s="19">
+      <c r="N38" s="11">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="O38" s="19">
+      <c r="O38" s="11">
         <f>E10</f>
         <v>0</v>
       </c>
-      <c r="P38" s="19">
+      <c r="P38" s="11">
         <f>E12</f>
         <v>0</v>
       </c>
-      <c r="Q38" s="19">
+      <c r="Q38" s="11">
         <f>E14</f>
         <v>0</v>
       </c>
-      <c r="R38" s="19">
+      <c r="R38" s="11">
         <f>E16</f>
-        <v>1</v>
-      </c>
-      <c r="S38" s="19">
+        <v>0</v>
+      </c>
+      <c r="S38" s="11">
         <f>E18</f>
-        <v>1.3</v>
-      </c>
-      <c r="T38" s="20">
+        <v>0</v>
+      </c>
+      <c r="T38" s="12">
         <f>E20</f>
         <v>0</v>
       </c>
       <c r="V38" t="s">
-        <v>14</v>
-      </c>
-      <c r="W38" s="23">
+        <v>12</v>
+      </c>
+      <c r="W38" s="15">
         <f>AVERAGE(J38:T48)</f>
-        <v>0.8672727272727272</v>
+        <v>3.2454545454545443</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -3156,66 +3152,66 @@
         <v>26</v>
       </c>
       <c r="C39">
-        <v>6.5</v>
+        <v>5.7</v>
       </c>
       <c r="D39">
-        <v>6.5</v>
+        <v>2.5</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="H39" s="14"/>
+      <c r="H39" s="19"/>
       <c r="I39" s="6">
         <f>A3</f>
         <v>26</v>
       </c>
-      <c r="J39" s="19">
+      <c r="J39" s="11">
         <f>$E3</f>
         <v>0</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="19">
+      <c r="K39" s="10"/>
+      <c r="L39" s="11">
         <f>E22</f>
         <v>0</v>
       </c>
-      <c r="M39" s="19">
+      <c r="M39" s="11">
         <f>E24</f>
-        <v>1.3</v>
-      </c>
-      <c r="N39" s="19">
+        <v>0</v>
+      </c>
+      <c r="N39" s="11">
         <f>E26</f>
         <v>0</v>
       </c>
-      <c r="O39" s="19">
+      <c r="O39" s="11">
         <f>E28</f>
         <v>0</v>
       </c>
-      <c r="P39" s="19">
+      <c r="P39" s="11">
         <f>E30</f>
         <v>0</v>
       </c>
-      <c r="Q39" s="19">
+      <c r="Q39" s="11">
         <f>E32</f>
-        <v>0.6</v>
-      </c>
-      <c r="R39" s="19">
+        <v>0</v>
+      </c>
+      <c r="R39" s="11">
         <f>E34</f>
-        <v>1</v>
-      </c>
-      <c r="S39" s="19">
+        <v>0</v>
+      </c>
+      <c r="S39" s="11">
         <f>E36</f>
-        <v>1.3</v>
-      </c>
-      <c r="T39" s="20">
+        <v>0</v>
+      </c>
+      <c r="T39" s="12">
         <f>E38</f>
         <v>0</v>
       </c>
       <c r="V39" t="s">
-        <v>15</v>
-      </c>
-      <c r="W39" s="24">
+        <v>13</v>
+      </c>
+      <c r="W39" s="16">
         <f>MAX(J38:T48)</f>
-        <v>10.6</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -3226,66 +3222,66 @@
         <v>77</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E40">
-        <v>3.9</v>
-      </c>
-      <c r="H40" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="19"/>
       <c r="I40" s="6">
         <f>A5</f>
         <v>51</v>
       </c>
-      <c r="J40" s="19">
+      <c r="J40" s="11">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="K40" s="19">
+      <c r="K40" s="11">
         <f>E23</f>
         <v>0</v>
       </c>
-      <c r="L40" s="18"/>
-      <c r="M40" s="19">
+      <c r="L40" s="10"/>
+      <c r="M40" s="11">
         <f>E40</f>
-        <v>3.9</v>
-      </c>
-      <c r="N40" s="19">
+        <v>0</v>
+      </c>
+      <c r="N40" s="11">
         <f>E42</f>
-        <v>1</v>
-      </c>
-      <c r="O40" s="19">
+        <v>0</v>
+      </c>
+      <c r="O40" s="11">
         <f>E44</f>
         <v>0</v>
       </c>
-      <c r="P40" s="19">
+      <c r="P40" s="11">
         <f>E46</f>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="11">
+        <f>E48</f>
         <v>0.6</v>
       </c>
-      <c r="Q40" s="19">
-        <f>E48</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="R40" s="19">
+      <c r="R40" s="11">
         <f>E50</f>
-        <v>1.5</v>
-      </c>
-      <c r="S40" s="19">
+        <v>0</v>
+      </c>
+      <c r="S40" s="11">
         <f>E52</f>
-        <v>1.7</v>
-      </c>
-      <c r="T40" s="20">
+        <v>0</v>
+      </c>
+      <c r="T40" s="12">
         <f>E54</f>
         <v>0</v>
       </c>
       <c r="V40" t="s">
-        <v>16</v>
-      </c>
-      <c r="W40" s="25">
+        <v>14</v>
+      </c>
+      <c r="W40" s="17">
         <f>((COUNTIF(J38:T48, "&gt;15"))/110)*100</f>
-        <v>0</v>
+        <v>7.2727272727272725</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -3296,57 +3292,57 @@
         <v>51</v>
       </c>
       <c r="C41">
-        <v>1.9</v>
+        <v>4.7</v>
       </c>
       <c r="D41">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="H41" s="14"/>
+        <v>13.3</v>
+      </c>
+      <c r="H41" s="19"/>
       <c r="I41" s="6">
         <f>A7</f>
         <v>77</v>
       </c>
-      <c r="J41" s="19">
+      <c r="J41" s="11">
         <f>E7</f>
         <v>0</v>
       </c>
-      <c r="K41" s="19">
+      <c r="K41" s="11">
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="L41" s="19">
+      <c r="L41" s="11">
         <f>E41</f>
-        <v>0</v>
-      </c>
-      <c r="M41" s="18"/>
-      <c r="N41" s="19">
+        <v>13.3</v>
+      </c>
+      <c r="M41" s="10"/>
+      <c r="N41" s="11">
         <f>E56</f>
-        <v>2</v>
-      </c>
-      <c r="O41" s="19">
+        <v>0</v>
+      </c>
+      <c r="O41" s="11">
         <f>E58</f>
-        <v>1.6</v>
-      </c>
-      <c r="P41" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="P41" s="11">
         <f>E60</f>
-        <v>1.3</v>
-      </c>
-      <c r="Q41" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="11">
         <f>E62</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="R41" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R41" s="11">
         <f>E64</f>
-        <v>1.5</v>
-      </c>
-      <c r="S41" s="19">
+        <v>0</v>
+      </c>
+      <c r="S41" s="11">
         <f>E66</f>
-        <v>1.7</v>
-      </c>
-      <c r="T41" s="20">
+        <v>0</v>
+      </c>
+      <c r="T41" s="12">
         <f>E68</f>
         <v>0</v>
       </c>
@@ -3359,57 +3355,57 @@
         <v>102</v>
       </c>
       <c r="C42">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>4.3</v>
+        <v>2.6</v>
       </c>
       <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="H42" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="19"/>
       <c r="I42" s="6">
         <f>A9</f>
         <v>102</v>
       </c>
-      <c r="J42" s="19">
+      <c r="J42" s="11">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="K42" s="19">
+      <c r="K42" s="11">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="L42" s="19">
+      <c r="L42" s="11">
         <f>E43</f>
-        <v>0</v>
-      </c>
-      <c r="M42" s="19">
+        <v>24.3</v>
+      </c>
+      <c r="M42" s="11">
         <f>E57</f>
-        <v>2.6</v>
-      </c>
-      <c r="N42" s="18"/>
-      <c r="O42" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="N42" s="10"/>
+      <c r="O42" s="11">
         <f>E70</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="P42" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="P42" s="11">
         <f>E72</f>
         <v>1.3</v>
       </c>
-      <c r="Q42" s="19">
+      <c r="Q42" s="11">
         <f>E74</f>
-        <v>1.7</v>
-      </c>
-      <c r="R42" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R42" s="11">
         <f>E76</f>
-        <v>2</v>
-      </c>
-      <c r="S42" s="19">
+        <v>0</v>
+      </c>
+      <c r="S42" s="11">
         <f>E78</f>
-        <v>1.7</v>
-      </c>
-      <c r="T42" s="20">
+        <v>0</v>
+      </c>
+      <c r="T42" s="12">
         <f>E80</f>
         <v>0</v>
       </c>
@@ -3422,57 +3418,57 @@
         <v>51</v>
       </c>
       <c r="C43">
-        <v>2.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="D43">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="H43" s="14"/>
+        <v>24.3</v>
+      </c>
+      <c r="H43" s="19"/>
       <c r="I43" s="6">
         <f>A11</f>
         <v>128</v>
       </c>
-      <c r="J43" s="19">
+      <c r="J43" s="11">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="K43" s="19">
+      <c r="K43" s="11">
         <f>E29</f>
         <v>0</v>
       </c>
-      <c r="L43" s="19">
+      <c r="L43" s="11">
         <f>E45</f>
-        <v>0</v>
-      </c>
-      <c r="M43" s="19">
+        <v>20.8</v>
+      </c>
+      <c r="M43" s="11">
         <f>E59</f>
-        <v>0</v>
-      </c>
-      <c r="N43" s="19">
+        <v>14.5</v>
+      </c>
+      <c r="N43" s="11">
         <f>E71</f>
-        <v>1</v>
-      </c>
-      <c r="O43" s="18"/>
-      <c r="P43" s="19">
+        <v>3.9</v>
+      </c>
+      <c r="O43" s="10"/>
+      <c r="P43" s="11">
         <f>E82</f>
-        <v>2</v>
-      </c>
-      <c r="Q43" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="Q43" s="11">
         <f>E84</f>
         <v>1.7</v>
       </c>
-      <c r="R43" s="19">
+      <c r="R43" s="11">
         <f>E86</f>
-        <v>2</v>
-      </c>
-      <c r="S43" s="19">
+        <v>0</v>
+      </c>
+      <c r="S43" s="11">
         <f>E88</f>
-        <v>1.7</v>
-      </c>
-      <c r="T43" s="20">
+        <v>0</v>
+      </c>
+      <c r="T43" s="12">
         <f>E90</f>
         <v>0</v>
       </c>
@@ -3485,57 +3481,57 @@
         <v>128</v>
       </c>
       <c r="C44">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="D44">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="H44" s="14"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="6">
         <f>A13</f>
         <v>153</v>
       </c>
-      <c r="J44" s="19">
+      <c r="J44" s="11">
         <f>E13</f>
         <v>0</v>
       </c>
-      <c r="K44" s="19">
+      <c r="K44" s="11">
         <f>E31</f>
         <v>0</v>
       </c>
-      <c r="L44" s="19">
+      <c r="L44" s="11">
         <f>E47</f>
-        <v>0</v>
-      </c>
-      <c r="M44" s="19">
+        <v>15.3</v>
+      </c>
+      <c r="M44" s="11">
         <f>E61</f>
-        <v>0</v>
-      </c>
-      <c r="N44" s="19">
+        <v>24.2</v>
+      </c>
+      <c r="N44" s="11">
         <f>E73</f>
-        <v>0</v>
-      </c>
-      <c r="O44" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="O44" s="11">
         <f>E83</f>
-        <v>1.6</v>
-      </c>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="19">
+        <v>3.1</v>
+      </c>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="11">
         <f>E92</f>
-        <v>1.7</v>
-      </c>
-      <c r="R44" s="19">
+        <v>0</v>
+      </c>
+      <c r="R44" s="11">
         <f>E94</f>
-        <v>2</v>
-      </c>
-      <c r="S44" s="19">
+        <v>0</v>
+      </c>
+      <c r="S44" s="11">
         <f>E96</f>
-        <v>1.7</v>
-      </c>
-      <c r="T44" s="20">
+        <v>0</v>
+      </c>
+      <c r="T44" s="12">
         <f>E98</f>
         <v>0</v>
       </c>
@@ -3548,57 +3544,57 @@
         <v>51</v>
       </c>
       <c r="C45">
-        <v>2.4</v>
+        <v>5.3</v>
       </c>
       <c r="D45">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="H45" s="14"/>
+        <v>20.8</v>
+      </c>
+      <c r="H45" s="19"/>
       <c r="I45" s="6">
         <f>A15</f>
         <v>179</v>
       </c>
-      <c r="J45" s="19">
+      <c r="J45" s="11">
         <f>E15</f>
         <v>0</v>
       </c>
-      <c r="K45" s="19">
+      <c r="K45" s="11">
         <f>E33</f>
         <v>0</v>
       </c>
-      <c r="L45" s="19">
+      <c r="L45" s="11">
         <f>E49</f>
-        <v>0</v>
-      </c>
-      <c r="M45" s="19">
+        <v>7.8</v>
+      </c>
+      <c r="M45" s="11">
         <f>E63</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="19">
+        <v>19.5</v>
+      </c>
+      <c r="N45" s="11">
         <f>E75</f>
-        <v>0</v>
-      </c>
-      <c r="O45" s="19">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="O45" s="11">
         <f>E85</f>
-        <v>0</v>
-      </c>
-      <c r="P45" s="19">
+        <v>7.2</v>
+      </c>
+      <c r="P45" s="11">
         <f>E93</f>
-        <v>1.3</v>
-      </c>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="19">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="11">
         <f>E100</f>
-        <v>2</v>
-      </c>
-      <c r="S45" s="19">
+        <v>0</v>
+      </c>
+      <c r="S45" s="11">
         <f>E102</f>
-        <v>1.7</v>
-      </c>
-      <c r="T45" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="T45" s="12">
         <f>E104</f>
         <v>0</v>
       </c>
@@ -3611,57 +3607,57 @@
         <v>153</v>
       </c>
       <c r="C46">
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
       <c r="D46">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="E46">
-        <v>0.6</v>
-      </c>
-      <c r="H46" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="19"/>
       <c r="I46" s="6">
         <f>A17</f>
         <v>204</v>
       </c>
-      <c r="J46" s="19">
+      <c r="J46" s="11">
         <f>E17</f>
         <v>0</v>
       </c>
-      <c r="K46" s="19">
+      <c r="K46" s="11">
         <f>E35</f>
         <v>0</v>
       </c>
-      <c r="L46" s="19">
+      <c r="L46" s="11">
         <f>E51</f>
         <v>0</v>
       </c>
-      <c r="M46" s="19">
+      <c r="M46" s="11">
         <f>E65</f>
-        <v>0</v>
-      </c>
-      <c r="N46" s="19">
+        <v>14</v>
+      </c>
+      <c r="N46" s="11">
         <f>E77</f>
-        <v>0</v>
-      </c>
-      <c r="O46" s="19">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="O46" s="11">
         <f>E87</f>
-        <v>0</v>
-      </c>
-      <c r="P46" s="19">
+        <v>12.5</v>
+      </c>
+      <c r="P46" s="11">
         <f>E95</f>
-        <v>0.6</v>
-      </c>
-      <c r="Q46" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="Q46" s="11">
         <f>E101</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="R46" s="18"/>
-      <c r="S46" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R46" s="10"/>
+      <c r="S46" s="11">
         <f>E106</f>
-        <v>1.7</v>
-      </c>
-      <c r="T46" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="T46" s="12">
         <f>E108</f>
         <v>0</v>
       </c>
@@ -3674,57 +3670,57 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>2.8</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="H47" s="14"/>
+        <v>15.3</v>
+      </c>
+      <c r="H47" s="19"/>
       <c r="I47" s="6">
         <f>A19</f>
         <v>230</v>
       </c>
-      <c r="J47" s="19">
+      <c r="J47" s="11">
         <f>E19</f>
         <v>0</v>
       </c>
-      <c r="K47" s="19">
+      <c r="K47" s="11">
         <f>E37</f>
         <v>0</v>
       </c>
-      <c r="L47" s="19">
+      <c r="L47" s="11">
         <f>E53</f>
         <v>0</v>
       </c>
-      <c r="M47" s="19">
+      <c r="M47" s="11">
         <f>E67</f>
-        <v>0</v>
-      </c>
-      <c r="N47" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="N47" s="11">
         <f>E79</f>
-        <v>0</v>
-      </c>
-      <c r="O47" s="19">
+        <v>14.5</v>
+      </c>
+      <c r="O47" s="11">
         <f>E89</f>
-        <v>0</v>
-      </c>
-      <c r="P47" s="19">
+        <v>17.7</v>
+      </c>
+      <c r="P47" s="11">
         <f>E97</f>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="19">
+        <v>11.2</v>
+      </c>
+      <c r="Q47" s="11">
         <f>E103</f>
-        <v>0.6</v>
-      </c>
-      <c r="R47" s="19">
+        <v>5.6</v>
+      </c>
+      <c r="R47" s="11">
         <f>E107</f>
-        <v>1</v>
-      </c>
-      <c r="S47" s="18"/>
-      <c r="T47" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="S47" s="10"/>
+      <c r="T47" s="12">
         <f>E110</f>
         <v>0</v>
       </c>
@@ -3740,57 +3736,57 @@
         <v>4.7</v>
       </c>
       <c r="D48">
-        <v>4.7</v>
+        <v>2.4</v>
       </c>
       <c r="E48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H48" s="15"/>
+        <v>0.6</v>
+      </c>
+      <c r="H48" s="20"/>
       <c r="I48" s="7">
         <f>A21</f>
         <v>255</v>
       </c>
-      <c r="J48" s="21">
+      <c r="J48" s="13">
         <f>E21</f>
         <v>0</v>
       </c>
-      <c r="K48" s="21">
+      <c r="K48" s="13">
         <f>E39</f>
         <v>0</v>
       </c>
-      <c r="L48" s="21">
+      <c r="L48" s="13">
         <f>E55</f>
         <v>0</v>
       </c>
-      <c r="M48" s="21">
+      <c r="M48" s="13">
         <f>E69</f>
         <v>0</v>
       </c>
-      <c r="N48" s="21">
+      <c r="N48" s="13">
         <f>E81</f>
-        <v>0</v>
-      </c>
-      <c r="O48" s="21">
+        <v>7.4</v>
+      </c>
+      <c r="O48" s="13">
         <f>E91</f>
-        <v>0</v>
-      </c>
-      <c r="P48" s="21">
+        <v>14.2</v>
+      </c>
+      <c r="P48" s="13">
         <f>E99</f>
-        <v>5</v>
-      </c>
-      <c r="Q48" s="21">
+        <v>12.7</v>
+      </c>
+      <c r="Q48" s="13">
         <f>E105</f>
-        <v>6.8</v>
-      </c>
-      <c r="R48" s="21">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R48" s="13">
         <f>E109</f>
-        <v>10.6</v>
-      </c>
-      <c r="S48" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="S48" s="13">
         <f>E111</f>
-        <v>6.6</v>
-      </c>
-      <c r="T48" s="22"/>
+        <v>0.9</v>
+      </c>
+      <c r="T48" s="14"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -3800,13 +3796,13 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="D49">
-        <v>2.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,13 +3813,13 @@
         <v>204</v>
       </c>
       <c r="C50">
-        <v>5.6</v>
+        <v>4.2</v>
       </c>
       <c r="D50">
-        <v>5.6</v>
+        <v>2.5</v>
       </c>
       <c r="E50">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,10 +3830,10 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="D51">
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -3851,13 +3847,13 @@
         <v>230</v>
       </c>
       <c r="C52">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="D52">
-        <v>5.8</v>
+        <v>2.6</v>
       </c>
       <c r="E52">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,10 +3864,10 @@
         <v>51</v>
       </c>
       <c r="C53">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="D53">
-        <v>3.5</v>
+        <v>2.4</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -3885,10 +3881,10 @@
         <v>255</v>
       </c>
       <c r="C54">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
       <c r="D54">
-        <v>4.9000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -3902,10 +3898,10 @@
         <v>51</v>
       </c>
       <c r="C55">
-        <v>5.9</v>
+        <v>5.4</v>
       </c>
       <c r="D55">
-        <v>5.9</v>
+        <v>2.5</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -3919,13 +3915,13 @@
         <v>102</v>
       </c>
       <c r="C56">
-        <v>4.9000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="D56">
-        <v>4.9000000000000004</v>
+        <v>2.1</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3936,13 +3932,13 @@
         <v>77</v>
       </c>
       <c r="C57">
-        <v>4.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="D57">
-        <v>4.0999999999999996</v>
+        <v>1.6</v>
       </c>
       <c r="E57">
-        <v>2.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3953,13 +3949,13 @@
         <v>128</v>
       </c>
       <c r="C58">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D58">
-        <v>4.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E58">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3970,13 +3966,13 @@
         <v>77</v>
       </c>
       <c r="C59">
-        <v>2.5</v>
+        <v>5.8</v>
       </c>
       <c r="D59">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3987,13 +3983,13 @@
         <v>153</v>
       </c>
       <c r="C60">
-        <v>4.5999999999999996</v>
+        <v>2.8</v>
       </c>
       <c r="D60">
-        <v>4.5999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="E60">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4004,13 +4000,13 @@
         <v>77</v>
       </c>
       <c r="C61">
-        <v>2.8</v>
+        <v>7</v>
       </c>
       <c r="D61">
-        <v>2.8</v>
+        <v>1.6</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4021,13 +4017,13 @@
         <v>179</v>
       </c>
       <c r="C62">
-        <v>5.0999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="D62">
-        <v>5.0999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="E62">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4038,13 +4034,13 @@
         <v>77</v>
       </c>
       <c r="C63">
-        <v>3.7</v>
+        <v>6.7</v>
       </c>
       <c r="D63">
-        <v>3.7</v>
+        <v>1.9</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4055,13 +4051,13 @@
         <v>204</v>
       </c>
       <c r="C64">
-        <v>5.6</v>
+        <v>3.7</v>
       </c>
       <c r="D64">
-        <v>5.6</v>
+        <v>2.5</v>
       </c>
       <c r="E64">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -4072,13 +4068,13 @@
         <v>77</v>
       </c>
       <c r="C65">
-        <v>3.9</v>
+        <v>6.3</v>
       </c>
       <c r="D65">
-        <v>3.9</v>
+        <v>2.1</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4089,13 +4085,13 @@
         <v>230</v>
       </c>
       <c r="C66">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="D66">
-        <v>5.6</v>
+        <v>2.7</v>
       </c>
       <c r="E66">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4106,13 +4102,13 @@
         <v>77</v>
       </c>
       <c r="C67">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
       <c r="D67">
-        <v>4.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4123,10 +4119,10 @@
         <v>255</v>
       </c>
       <c r="C68">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
       <c r="D68">
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -4140,10 +4136,10 @@
         <v>77</v>
       </c>
       <c r="C69">
-        <v>6.6</v>
+        <v>3.7</v>
       </c>
       <c r="D69">
-        <v>6.6</v>
+        <v>2.4</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -4157,13 +4153,13 @@
         <v>128</v>
       </c>
       <c r="C70">
-        <v>5.3</v>
+        <v>4.5</v>
       </c>
       <c r="D70">
-        <v>5.3</v>
+        <v>2.1</v>
       </c>
       <c r="E70">
-        <v>2.2999999999999998</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4174,13 +4170,13 @@
         <v>102</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>1.9</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4191,10 +4187,10 @@
         <v>153</v>
       </c>
       <c r="C72">
-        <v>5.0999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="D72">
-        <v>5.0999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E72">
         <v>1.3</v>
@@ -4208,13 +4204,13 @@
         <v>102</v>
       </c>
       <c r="C73">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="D73">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4225,13 +4221,13 @@
         <v>179</v>
       </c>
       <c r="C74">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
       <c r="D74">
-        <v>5.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E74">
-        <v>1.7</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4242,13 +4238,13 @@
         <v>102</v>
       </c>
       <c r="C75">
-        <v>2.9</v>
+        <v>7.4</v>
       </c>
       <c r="D75">
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,13 +4255,13 @@
         <v>204</v>
       </c>
       <c r="C76">
-        <v>5.6</v>
+        <v>4.3</v>
       </c>
       <c r="D76">
-        <v>5.6</v>
+        <v>2.5</v>
       </c>
       <c r="E76">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,13 +4272,13 @@
         <v>102</v>
       </c>
       <c r="C77">
-        <v>4.8</v>
+        <v>7.6</v>
       </c>
       <c r="D77">
-        <v>4.8</v>
+        <v>1.7</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -4293,13 +4289,13 @@
         <v>230</v>
       </c>
       <c r="C78">
-        <v>5.7</v>
+        <v>4.2</v>
       </c>
       <c r="D78">
-        <v>5.7</v>
+        <v>2.6</v>
       </c>
       <c r="E78">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4310,13 +4306,13 @@
         <v>102</v>
       </c>
       <c r="C79">
-        <v>5.5</v>
+        <v>7.3</v>
       </c>
       <c r="D79">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4327,10 +4323,10 @@
         <v>255</v>
       </c>
       <c r="C80">
-        <v>4.8</v>
+        <v>5.7</v>
       </c>
       <c r="D80">
-        <v>4.8</v>
+        <v>2.6</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -4344,13 +4340,13 @@
         <v>102</v>
       </c>
       <c r="C81">
-        <v>5.9</v>
+        <v>6.5</v>
       </c>
       <c r="D81">
-        <v>5.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4361,13 +4357,13 @@
         <v>153</v>
       </c>
       <c r="C82">
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
       <c r="D82">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E82">
-        <v>2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4378,13 +4374,13 @@
         <v>128</v>
       </c>
       <c r="C83">
-        <v>4.3</v>
+        <v>5.2</v>
       </c>
       <c r="D83">
-        <v>4.3</v>
+        <v>1.8</v>
       </c>
       <c r="E83">
-        <v>1.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4395,10 +4391,10 @@
         <v>179</v>
       </c>
       <c r="C84">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="D84">
-        <v>5.4</v>
+        <v>2</v>
       </c>
       <c r="E84">
         <v>1.7</v>
@@ -4412,13 +4408,13 @@
         <v>128</v>
       </c>
       <c r="C85">
-        <v>2.5</v>
+        <v>7.2</v>
       </c>
       <c r="D85">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4429,13 +4425,13 @@
         <v>204</v>
       </c>
       <c r="C86">
-        <v>5.7</v>
+        <v>3.6</v>
       </c>
       <c r="D86">
-        <v>5.7</v>
+        <v>2.4</v>
       </c>
       <c r="E86">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4446,13 +4442,13 @@
         <v>128</v>
       </c>
       <c r="C87">
-        <v>2.7</v>
+        <v>7.7</v>
       </c>
       <c r="D87">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4463,13 +4459,13 @@
         <v>230</v>
       </c>
       <c r="C88">
-        <v>5.6</v>
+        <v>3.5</v>
       </c>
       <c r="D88">
-        <v>5.6</v>
+        <v>2.5</v>
       </c>
       <c r="E88">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4480,13 +4476,13 @@
         <v>128</v>
       </c>
       <c r="C89">
-        <v>3.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D89">
-        <v>3.9</v>
+        <v>1.7</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>17.7</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4497,10 +4493,10 @@
         <v>255</v>
       </c>
       <c r="C90">
-        <v>4.5999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D90">
-        <v>4.5999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -4514,13 +4510,13 @@
         <v>128</v>
       </c>
       <c r="C91">
-        <v>2.8</v>
+        <v>7.6</v>
       </c>
       <c r="D91">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4531,13 +4527,13 @@
         <v>179</v>
       </c>
       <c r="C92">
-        <v>5.4</v>
+        <v>2.6</v>
       </c>
       <c r="D92">
-        <v>5.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E92">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4548,13 +4544,13 @@
         <v>153</v>
       </c>
       <c r="C93">
-        <v>4.3</v>
+        <v>5.2</v>
       </c>
       <c r="D93">
-        <v>4.3</v>
+        <v>1.9</v>
       </c>
       <c r="E93">
-        <v>1.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -4565,13 +4561,13 @@
         <v>204</v>
       </c>
       <c r="C94">
-        <v>5.5</v>
+        <v>2.8</v>
       </c>
       <c r="D94">
-        <v>5.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E94">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4582,13 +4578,13 @@
         <v>153</v>
       </c>
       <c r="C95">
-        <v>4.2</v>
+        <v>7.1</v>
       </c>
       <c r="D95">
-        <v>4.2</v>
+        <v>1.7</v>
       </c>
       <c r="E95">
-        <v>0.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4599,13 +4595,13 @@
         <v>230</v>
       </c>
       <c r="C96">
-        <v>5.6</v>
+        <v>4.5</v>
       </c>
       <c r="D96">
-        <v>5.6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E96">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4616,13 +4612,13 @@
         <v>153</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>7.8</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4633,10 +4629,10 @@
         <v>255</v>
       </c>
       <c r="C98">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="D98">
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -4650,13 +4646,13 @@
         <v>153</v>
       </c>
       <c r="C99">
-        <v>6.3</v>
+        <v>7.8</v>
       </c>
       <c r="D99">
-        <v>6.3</v>
+        <v>1.7</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4667,13 +4663,13 @@
         <v>204</v>
       </c>
       <c r="C100">
-        <v>5.4</v>
+        <v>2.6</v>
       </c>
       <c r="D100">
-        <v>5.4</v>
+        <v>2.1</v>
       </c>
       <c r="E100">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4684,13 +4680,13 @@
         <v>179</v>
       </c>
       <c r="C101">
-        <v>4.3</v>
+        <v>6.4</v>
       </c>
       <c r="D101">
-        <v>4.3</v>
+        <v>1.7</v>
       </c>
       <c r="E101">
-        <v>1.1000000000000001</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4701,13 +4697,13 @@
         <v>230</v>
       </c>
       <c r="C102">
-        <v>5.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D102">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E102">
-        <v>1.7</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4718,13 +4714,13 @@
         <v>179</v>
       </c>
       <c r="C103">
-        <v>4.0999999999999996</v>
+        <v>7.1</v>
       </c>
       <c r="D103">
-        <v>4.0999999999999996</v>
+        <v>1.6</v>
       </c>
       <c r="E103">
-        <v>0.6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4738,7 +4734,7 @@
         <v>4.5</v>
       </c>
       <c r="D104">
-        <v>4.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -4752,13 +4748,13 @@
         <v>179</v>
       </c>
       <c r="C105">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="D105">
-        <v>6.7</v>
+        <v>1.7</v>
       </c>
       <c r="E105">
-        <v>6.8</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4769,13 +4765,13 @@
         <v>230</v>
       </c>
       <c r="C106">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="D106">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E106">
-        <v>1.7</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4786,13 +4782,13 @@
         <v>204</v>
       </c>
       <c r="C107">
-        <v>4.5999999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="D107">
-        <v>4.5999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4803,10 +4799,10 @@
         <v>255</v>
       </c>
       <c r="C108">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="D108">
-        <v>3.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -4820,13 +4816,13 @@
         <v>204</v>
       </c>
       <c r="C109">
-        <v>7</v>
+        <v>6.3</v>
       </c>
       <c r="D109">
-        <v>7</v>
+        <v>1.9</v>
       </c>
       <c r="E109">
-        <v>10.6</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4837,10 +4833,10 @@
         <v>255</v>
       </c>
       <c r="C110">
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
       <c r="D110">
-        <v>3.6</v>
+        <v>2.5</v>
       </c>
       <c r="E110">
         <v>0</v>
@@ -4854,26 +4850,26 @@
         <v>230</v>
       </c>
       <c r="C111">
-        <v>6.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D111">
-        <v>6.4</v>
+        <v>1.9</v>
       </c>
       <c r="E111">
-        <v>6.6</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H38:H48"/>
+    <mergeCell ref="H5:H15"/>
+    <mergeCell ref="J3:T3"/>
+    <mergeCell ref="H34:L34"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="J20:T20"/>
     <mergeCell ref="H22:H32"/>
     <mergeCell ref="H18:L18"/>
     <mergeCell ref="J36:T36"/>
-    <mergeCell ref="H38:H48"/>
-    <mergeCell ref="H5:H15"/>
-    <mergeCell ref="J3:T3"/>
-    <mergeCell ref="H34:L34"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:T15 W7:W9 W24:W27 J22:T32 W11:W12 W29:W30">
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
Updates to templates, added circuit diagram, uploaded arduino libraries required just in case.
</commit_message>
<xml_diff>
--- a/Results Template.xlsx
+++ b/Results Template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
   <si>
     <t>Starting RGB</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Input Lag (ms)</t>
-  </si>
-  <si>
-    <t>CHANGE THIS</t>
   </si>
 </sst>
 </file>
@@ -1015,216 +1012,111 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1243,20 +1135,125 @@
     <xf numFmtId="0" fontId="22" fillId="38" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2476,13 +2473,13 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2490,13 +2487,13 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="47" t="s">
+      <c r="N2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -2504,13 +2501,13 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="47" t="s">
+      <c r="Z2" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="47"/>
-      <c r="AD2" s="47"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
@@ -2560,14 +2557,14 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="4"/>
       <c r="K4" s="8" t="s">
         <v>3</v>
@@ -2578,14 +2575,14 @@
       <c r="M4" s="4"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
+      <c r="P4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
       <c r="V4" s="4"/>
       <c r="W4" s="8" t="s">
         <v>3</v>
@@ -2597,14 +2594,14 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
+      <c r="AB4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50"/>
       <c r="AH4" s="4"/>
       <c r="AI4" s="8" t="s">
         <v>3</v>
@@ -2723,7 +2720,7 @@
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
@@ -2760,7 +2757,7 @@
         <v>100</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="51" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="1">
@@ -2797,7 +2794,7 @@
         <v>100</v>
       </c>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="52" t="s">
+      <c r="Z6" s="51" t="s">
         <v>2</v>
       </c>
       <c r="AA6" s="1">
@@ -2836,7 +2833,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="52"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2866,7 +2863,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="52"/>
+      <c r="N7" s="51"/>
       <c r="O7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2896,7 +2893,7 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="52"/>
+      <c r="Z7" s="51"/>
       <c r="AA7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2928,7 +2925,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="52"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -2963,7 +2960,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="52"/>
+      <c r="N8" s="51"/>
       <c r="O8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -2998,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="52"/>
+      <c r="Z8" s="51"/>
       <c r="AA8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -3035,7 +3032,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="52"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3070,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="52"/>
+      <c r="N9" s="51"/>
       <c r="O9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3105,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="52"/>
+      <c r="Z9" s="51"/>
       <c r="AA9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3142,7 +3139,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="52"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3177,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="52"/>
+      <c r="N10" s="51"/>
       <c r="O10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3212,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="52"/>
+      <c r="Z10" s="51"/>
       <c r="AA10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3249,7 +3246,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="52"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3284,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="3"/>
-      <c r="N11" s="52"/>
+      <c r="N11" s="51"/>
       <c r="O11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3319,7 +3316,7 @@
         <v>2</v>
       </c>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="52"/>
+      <c r="Z11" s="51"/>
       <c r="AA11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3602,13 +3599,13 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -3616,13 +3613,13 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="47" t="s">
+      <c r="N19" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="47"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
       <c r="S19" s="1"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -3662,14 +3659,14 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
+      <c r="D21" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
       <c r="J21" s="4"/>
       <c r="K21" s="8" t="s">
         <v>15</v>
@@ -3680,14 +3677,14 @@
       <c r="M21" s="4"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
+      <c r="P21" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
       <c r="V21" s="4"/>
       <c r="W21" s="8" t="s">
         <v>3</v>
@@ -3697,15 +3694,15 @@
         <v>60</v>
       </c>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="58" t="s">
+      <c r="Z21" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="AA21" s="60"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
-      <c r="AE21" s="60"/>
-      <c r="AF21" s="59"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="57"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -3774,23 +3771,23 @@
         <v>16.666666666666668</v>
       </c>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="58" t="s">
+      <c r="Z22" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="AA22" s="60"/>
-      <c r="AB22" s="60"/>
-      <c r="AC22" s="59"/>
-      <c r="AD22" s="58" t="s">
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58"/>
+      <c r="AC22" s="57"/>
+      <c r="AD22" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="AE22" s="59"/>
+      <c r="AE22" s="57"/>
       <c r="AF22" s="41" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="1">
@@ -3827,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="3"/>
-      <c r="N23" s="52" t="s">
+      <c r="N23" s="51" t="s">
         <v>2</v>
       </c>
       <c r="O23" s="1">
@@ -3864,16 +3861,16 @@
         <v>100</v>
       </c>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="61" t="s">
+      <c r="Z23" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="AA23" s="62"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="63"/>
-      <c r="AD23" s="64">
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="61"/>
+      <c r="AD23" s="62">
         <v>0.33</v>
       </c>
-      <c r="AE23" s="63"/>
+      <c r="AE23" s="61"/>
       <c r="AF23" s="42">
         <f>100-$X$26</f>
         <v>99</v>
@@ -3881,7 +3878,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="52"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -3916,7 +3913,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="3"/>
-      <c r="N24" s="52"/>
+      <c r="N24" s="51"/>
       <c r="O24" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -3946,16 +3943,16 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="46" t="s">
+      <c r="Z24" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="AA24" s="47"/>
-      <c r="AB24" s="47"/>
-      <c r="AC24" s="48"/>
-      <c r="AD24" s="65">
+      <c r="AA24" s="50"/>
+      <c r="AB24" s="50"/>
+      <c r="AC24" s="64"/>
+      <c r="AD24" s="63">
         <v>0.33</v>
       </c>
-      <c r="AE24" s="48"/>
+      <c r="AE24" s="64"/>
       <c r="AF24" s="43">
         <f>100-$L$9</f>
         <v>99</v>
@@ -3963,7 +3960,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="52"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -3998,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3"/>
-      <c r="N25" s="52"/>
+      <c r="N25" s="51"/>
       <c r="O25" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -4033,16 +4030,16 @@
         <v>1</v>
       </c>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="46" t="s">
+      <c r="Z25" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="AA25" s="47"/>
-      <c r="AB25" s="47"/>
-      <c r="AC25" s="48"/>
-      <c r="AD25" s="65">
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="50"/>
+      <c r="AC25" s="64"/>
+      <c r="AD25" s="63">
         <v>0.1</v>
       </c>
-      <c r="AE25" s="48"/>
+      <c r="AE25" s="64"/>
       <c r="AF25" s="43">
         <f>100-$L$10</f>
         <v>99</v>
@@ -4050,7 +4047,7 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="52"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -4080,7 +4077,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="52"/>
+      <c r="N26" s="51"/>
       <c r="O26" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -4115,16 +4112,16 @@
         <v>1</v>
       </c>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="46" t="s">
+      <c r="Z26" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="AA26" s="47"/>
-      <c r="AB26" s="47"/>
-      <c r="AC26" s="48"/>
-      <c r="AD26" s="65">
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="50"/>
+      <c r="AC26" s="64"/>
+      <c r="AD26" s="63">
         <v>0.1</v>
       </c>
-      <c r="AE26" s="48"/>
+      <c r="AE26" s="64"/>
       <c r="AF26" s="43">
         <f>100-$L$11</f>
         <v>99</v>
@@ -4132,7 +4129,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="52"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -4162,7 +4159,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="52"/>
+      <c r="N27" s="51"/>
       <c r="O27" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -4197,16 +4194,16 @@
         <v>1</v>
       </c>
       <c r="Y27" s="3"/>
-      <c r="Z27" s="46" t="s">
+      <c r="Z27" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="AA27" s="47"/>
-      <c r="AB27" s="47"/>
-      <c r="AC27" s="48"/>
-      <c r="AD27" s="65">
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="50"/>
+      <c r="AC27" s="64"/>
+      <c r="AD27" s="63">
         <v>0.1</v>
       </c>
-      <c r="AE27" s="48"/>
+      <c r="AE27" s="64"/>
       <c r="AF27" s="43">
         <f>100-$L$23</f>
         <v>99</v>
@@ -4214,7 +4211,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="52"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -4244,7 +4241,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="52"/>
+      <c r="N28" s="51"/>
       <c r="O28" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -4279,16 +4276,16 @@
         <v>1</v>
       </c>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="49" t="s">
+      <c r="Z28" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="AA28" s="50"/>
-      <c r="AB28" s="50"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="66">
+      <c r="AA28" s="70"/>
+      <c r="AB28" s="70"/>
+      <c r="AC28" s="66"/>
+      <c r="AD28" s="65">
         <v>0.04</v>
       </c>
-      <c r="AE28" s="51"/>
+      <c r="AE28" s="66"/>
       <c r="AF28" s="44">
         <f>100-$L$5</f>
         <v>83.333333333333329</v>
@@ -4325,11 +4322,11 @@
         <v>2</v>
       </c>
       <c r="Y29" s="6"/>
-      <c r="AC29" s="55" t="s">
+      <c r="AC29" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="AD29" s="56"/>
-      <c r="AE29" s="57"/>
+      <c r="AD29" s="54"/>
+      <c r="AE29" s="55"/>
       <c r="AF29" s="45">
         <f>(($AF$23*$AD$23)+($AF$24*$AD$24)+($AF$25*$AD$25)+($AF$26*$AD$26)+($AF$27*$AD$27)+($AF$28*$AD$28))/10</f>
         <v>9.8373333333333353</v>
@@ -4401,23 +4398,23 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
       <c r="I32" s="12"/>
-      <c r="J32" s="54" t="s">
+      <c r="J32" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
       <c r="M32" s="6"/>
       <c r="N32" s="5"/>
       <c r="O32" s="1"/>
@@ -4560,6 +4557,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="Z24:AC24"/>
+    <mergeCell ref="Z25:AC25"/>
+    <mergeCell ref="Z26:AC26"/>
+    <mergeCell ref="Z27:AC27"/>
+    <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="P21:U21"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="N23:N28"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="N6:N11"/>
     <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AB4:AG4"/>
     <mergeCell ref="Z6:Z11"/>
@@ -4576,24 +4591,6 @@
     <mergeCell ref="AD26:AE26"/>
     <mergeCell ref="AD27:AE27"/>
     <mergeCell ref="AD28:AE28"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="P21:U21"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="N23:N28"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z25:AC25"/>
-    <mergeCell ref="Z26:AC26"/>
-    <mergeCell ref="Z27:AC27"/>
-    <mergeCell ref="Z28:AC28"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:I11 P6:U11 P23:U28 L8:L11 L13:L14 X8:X10 X12:X13 X25:X28 X30:X31">
     <cfRule type="colorScale" priority="10">
@@ -4643,7 +4640,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 X6 X23">
+  <conditionalFormatting sqref="X6 L6 X23">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="50"/>
@@ -4738,7 +4735,7 @@
   <dimension ref="A1:AR58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:R13"/>
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4802,42 +4799,42 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="108" t="str">
         <f>'PASTE DATA HERE'!$E$1</f>
         <v>Perceived Response Time - RGB5 (ms)</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="110"/>
       <c r="J2" s="31"/>
-      <c r="K2" s="70" t="str">
+      <c r="K2" s="108" t="str">
         <f>'PASTE DATA HERE'!$F$1</f>
         <v>Overshoot (RGB)</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="72"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="110"/>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
-      <c r="U2" s="70" t="str">
+      <c r="U2" s="108" t="str">
         <f>'PASTE DATA HERE'!$G$1</f>
         <v>Visual Response Rating</v>
       </c>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="72"/>
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="109"/>
+      <c r="AB2" s="110"/>
       <c r="AC2" s="31"/>
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
@@ -4905,37 +4902,37 @@
       <c r="A4" s="30"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
-      <c r="D4" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="57"/>
       <c r="J4" s="32"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
-      <c r="M4" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="59"/>
+      <c r="M4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="57"/>
       <c r="S4" s="32"/>
       <c r="T4" s="30"/>
       <c r="U4" s="31"/>
       <c r="V4" s="31"/>
-      <c r="W4" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="Z4" s="60"/>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="59"/>
+      <c r="W4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="57"/>
       <c r="AC4" s="32"/>
       <c r="AD4" s="34"/>
       <c r="AE4" s="33"/>
@@ -5055,7 +5052,7 @@
     </row>
     <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="114" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="25">
@@ -5084,7 +5081,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="33"/>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="114" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="25">
@@ -5114,7 +5111,7 @@
       </c>
       <c r="S6" s="33"/>
       <c r="T6" s="30"/>
-      <c r="U6" s="67" t="s">
+      <c r="U6" s="114" t="s">
         <v>2</v>
       </c>
       <c r="V6" s="25">
@@ -5161,7 +5158,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="68"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5188,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="33"/>
-      <c r="K7" s="68"/>
+      <c r="K7" s="115"/>
       <c r="L7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5216,7 +5213,7 @@
       </c>
       <c r="S7" s="33"/>
       <c r="T7" s="30"/>
-      <c r="U7" s="68"/>
+      <c r="U7" s="115"/>
       <c r="V7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5261,7 +5258,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="68"/>
+      <c r="B8" s="115"/>
       <c r="C8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5288,7 +5285,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="33"/>
-      <c r="K8" s="68"/>
+      <c r="K8" s="115"/>
       <c r="L8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5316,7 +5313,7 @@
       </c>
       <c r="S8" s="33"/>
       <c r="T8" s="30"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="115"/>
       <c r="V8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5361,7 +5358,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
-      <c r="B9" s="68"/>
+      <c r="B9" s="115"/>
       <c r="C9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5388,7 +5385,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="33"/>
-      <c r="K9" s="68"/>
+      <c r="K9" s="115"/>
       <c r="L9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5416,7 +5413,7 @@
       </c>
       <c r="S9" s="33"/>
       <c r="T9" s="33"/>
-      <c r="U9" s="68"/>
+      <c r="U9" s="115"/>
       <c r="V9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5461,7 +5458,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="68"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5488,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="33"/>
-      <c r="K10" s="68"/>
+      <c r="K10" s="115"/>
       <c r="L10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5516,7 +5513,7 @@
       </c>
       <c r="S10" s="33"/>
       <c r="T10" s="33"/>
-      <c r="U10" s="68"/>
+      <c r="U10" s="115"/>
       <c r="V10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5561,7 +5558,7 @@
     </row>
     <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
-      <c r="B11" s="69"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5588,7 +5585,7 @@
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="33"/>
-      <c r="K11" s="69"/>
+      <c r="K11" s="116"/>
       <c r="L11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5616,7 +5613,7 @@
       <c r="R11" s="24"/>
       <c r="S11" s="33"/>
       <c r="T11" s="33"/>
-      <c r="U11" s="69"/>
+      <c r="U11" s="116"/>
       <c r="V11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5708,46 +5705,47 @@
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="88">
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="103">
         <f>'VIEW HEATMAPS HERE'!L4</f>
         <v>60</v>
       </c>
-      <c r="I13" s="90"/>
+      <c r="I13" s="104"/>
       <c r="J13" s="33"/>
       <c r="K13" s="30"/>
-      <c r="L13" s="88" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
+      <c r="L13" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
       <c r="O13" s="90"/>
-      <c r="P13" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="90"/>
+      <c r="P13" s="90"/>
+      <c r="Q13" s="92">
+        <f>AVERAGE(M6:R11)</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="93"/>
       <c r="S13" s="30"/>
       <c r="T13" s="30"/>
       <c r="U13" s="30"/>
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
-      <c r="X13" s="86" t="s">
+      <c r="X13" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="Y13" s="87"/>
-      <c r="Z13" s="94"/>
-      <c r="AA13" s="82">
+      <c r="Y13" s="90"/>
+      <c r="Z13" s="91"/>
+      <c r="AA13" s="92">
         <f>AVERAGE(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB13" s="83"/>
+      <c r="AB13" s="93"/>
       <c r="AC13" s="30"/>
       <c r="AD13" s="30"/>
       <c r="AE13" s="30"/>
@@ -5768,42 +5766,47 @@
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="97">
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="105">
         <f>1000/$H$13</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="I14" s="98"/>
+      <c r="I14" s="106"/>
       <c r="J14" s="33"/>
       <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="31"/>
+      <c r="L14" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="101">
+        <f>MAX(M6:R11)</f>
+        <v>1</v>
+      </c>
+      <c r="R14" s="102"/>
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
-      <c r="X14" s="91" t="s">
+      <c r="X14" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="92"/>
-      <c r="Z14" s="93"/>
-      <c r="AA14" s="95">
+      <c r="Y14" s="72"/>
+      <c r="Z14" s="73"/>
+      <c r="AA14" s="94">
         <f>AVERAGE(X6:AB6,Y7:AB7,Z8:AB8,AA9:AB9,AB10)</f>
         <v>1</v>
       </c>
-      <c r="AB14" s="96"/>
+      <c r="AB14" s="95"/>
       <c r="AC14" s="30"/>
       <c r="AD14" s="30"/>
       <c r="AE14" s="30"/>
@@ -5824,47 +5827,47 @@
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="99">
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="127">
         <f>((COUNTIF(D6:I11, "&lt;" &amp;H14))/COUNT(D6:I11))*100</f>
         <v>100</v>
       </c>
-      <c r="I15" s="100"/>
+      <c r="I15" s="128"/>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="82">
-        <f>AVERAGE(M6:R11)</f>
-        <v>1</v>
-      </c>
-      <c r="R15" s="83"/>
+      <c r="L15" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="77">
+        <f>((COUNTIF(M6:R11, "&gt;15"))/COUNT(M6:R11))*100</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="78"/>
       <c r="S15" s="30"/>
       <c r="T15" s="30"/>
       <c r="U15" s="30"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
-      <c r="X15" s="91" t="s">
+      <c r="X15" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="Y15" s="92"/>
-      <c r="Z15" s="93"/>
-      <c r="AA15" s="95">
+      <c r="Y15" s="72"/>
+      <c r="Z15" s="73"/>
+      <c r="AA15" s="94">
         <f>AVERAGE(W7:W11,X8:X11,Y9:Y11,Z10:Z11,AA11)</f>
         <v>1</v>
       </c>
-      <c r="AB15" s="96"/>
+      <c r="AB15" s="95"/>
       <c r="AC15" s="30"/>
       <c r="AD15" s="30"/>
       <c r="AE15" s="30"/>
@@ -5894,33 +5897,28 @@
       <c r="I16" s="31"/>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="84">
-        <f>MAX(M6:R11)</f>
-        <v>1</v>
-      </c>
-      <c r="R16" s="85"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
       <c r="S16" s="30"/>
       <c r="T16" s="30"/>
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
-      <c r="X16" s="91" t="s">
+      <c r="X16" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="Y16" s="92"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="84">
+      <c r="Y16" s="72"/>
+      <c r="Z16" s="73"/>
+      <c r="AA16" s="101">
         <f>AB6+W11</f>
         <v>2</v>
       </c>
-      <c r="AB16" s="85"/>
+      <c r="AB16" s="102"/>
       <c r="AC16" s="30"/>
       <c r="AD16" s="30"/>
       <c r="AE16" s="30"/>
@@ -5941,47 +5939,42 @@
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="82">
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="92">
         <f>'VIEW HEATMAPS HERE'!$X$26</f>
         <v>1</v>
       </c>
-      <c r="I17" s="83"/>
+      <c r="I17" s="93"/>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="113">
-        <f>((COUNTIF(M6:R11, "&gt;15"))/COUNT(M6:R11))*100</f>
-        <v>0</v>
-      </c>
-      <c r="R17" s="114"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
       <c r="S17" s="30"/>
       <c r="T17" s="30"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
       <c r="W17" s="30"/>
-      <c r="X17" s="91" t="s">
+      <c r="X17" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="Y17" s="92"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="84">
+      <c r="Y17" s="72"/>
+      <c r="Z17" s="73"/>
+      <c r="AA17" s="101">
         <f>MIN(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB17" s="85"/>
+      <c r="AB17" s="102"/>
       <c r="AC17" s="30"/>
       <c r="AD17" s="30"/>
       <c r="AE17" s="30"/>
@@ -6002,18 +5995,18 @@
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="95">
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="94">
         <f>'VIEW HEATMAPS HERE'!$X$8</f>
         <v>1</v>
       </c>
-      <c r="I18" s="96"/>
+      <c r="I18" s="95"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -6028,16 +6021,16 @@
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
-      <c r="X18" s="73" t="s">
+      <c r="X18" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="Y18" s="74"/>
-      <c r="Z18" s="75"/>
-      <c r="AA18" s="101">
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="76"/>
+      <c r="AA18" s="99">
         <f>MAX(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB18" s="102"/>
+      <c r="AB18" s="100"/>
       <c r="AC18" s="30"/>
       <c r="AD18" s="30"/>
       <c r="AE18" s="30"/>
@@ -6058,18 +6051,18 @@
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="30"/>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="95">
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="94">
         <f>AVERAGE(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I19" s="96"/>
+      <c r="I19" s="95"/>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -6109,32 +6102,32 @@
     <row r="20" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="30"/>
-      <c r="C20" s="91" t="s">
+      <c r="C20" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="95">
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="94">
         <f>AVERAGE(E6:I6,F7:I7,G8:I8,H9:I9,I10)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="96"/>
+      <c r="I20" s="95"/>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
-      <c r="M20" s="76" t="s">
+      <c r="M20" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="77"/>
-      <c r="O20" s="78"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="113"/>
       <c r="P20" s="30"/>
-      <c r="Q20" s="79" t="s">
+      <c r="Q20" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="R20" s="80"/>
-      <c r="S20" s="81"/>
+      <c r="R20" s="97"/>
+      <c r="S20" s="98"/>
       <c r="T20" s="30"/>
       <c r="U20" s="30"/>
       <c r="V20" s="30"/>
@@ -6164,18 +6157,18 @@
     <row r="21" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="91" t="s">
+      <c r="C21" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="92"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="92"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="95">
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="94">
         <f>AVERAGE(D7:D11,E8:E11,F9:F11,G10:G11,H11)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="96"/>
+      <c r="I21" s="95"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -6201,17 +6194,17 @@
       <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="1"/>
-      <c r="W21" s="118" t="s">
+      <c r="W21" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="X21" s="119"/>
-      <c r="Y21" s="119"/>
-      <c r="Z21" s="120"/>
-      <c r="AA21" s="124">
+      <c r="X21" s="84"/>
+      <c r="Y21" s="84"/>
+      <c r="Z21" s="85"/>
+      <c r="AA21" s="79">
         <f>AVERAGE('PASTE DATA HERE'!H2:H31)</f>
         <v>1</v>
       </c>
-      <c r="AB21" s="125"/>
+      <c r="AB21" s="80"/>
       <c r="AC21" s="30"/>
       <c r="AD21" s="30"/>
       <c r="AE21" s="30"/>
@@ -6232,18 +6225,18 @@
     <row r="22" spans="1:44" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="30"/>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="84">
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="101">
         <f>I6+D11</f>
         <v>2</v>
       </c>
-      <c r="I22" s="85"/>
+      <c r="I22" s="102"/>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
@@ -6256,13 +6249,13 @@
       <c r="S22" s="30"/>
       <c r="T22" s="30"/>
       <c r="U22" s="30"/>
-      <c r="V22" s="128"/>
-      <c r="W22" s="121"/>
-      <c r="X22" s="122"/>
-      <c r="Y22" s="122"/>
-      <c r="Z22" s="123"/>
-      <c r="AA22" s="126"/>
-      <c r="AB22" s="127"/>
+      <c r="V22" s="49"/>
+      <c r="W22" s="86"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="87"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="81"/>
+      <c r="AB22" s="82"/>
       <c r="AC22" s="30"/>
       <c r="AD22" s="30"/>
       <c r="AE22" s="30"/>
@@ -6283,46 +6276,46 @@
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="91" t="s">
+      <c r="C23" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="84">
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="101">
         <f>MIN(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="85"/>
+      <c r="I23" s="102"/>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="79" t="s">
+      <c r="M23" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="80"/>
-      <c r="O23" s="81"/>
+      <c r="N23" s="97"/>
+      <c r="O23" s="98"/>
       <c r="P23" s="30"/>
-      <c r="Q23" s="61" t="s">
+      <c r="Q23" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="R23" s="62"/>
-      <c r="S23" s="63"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="61"/>
       <c r="T23" s="30"/>
       <c r="U23" s="30"/>
       <c r="V23" s="30"/>
-      <c r="W23" s="103" t="s">
+      <c r="W23" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="X23" s="104"/>
-      <c r="Y23" s="104"/>
-      <c r="Z23" s="105"/>
-      <c r="AA23" s="109">
+      <c r="X23" s="118"/>
+      <c r="Y23" s="118"/>
+      <c r="Z23" s="119"/>
+      <c r="AA23" s="123">
         <f>'VIEW HEATMAPS HERE'!$AF$29</f>
         <v>9.8373333333333353</v>
       </c>
-      <c r="AB23" s="110"/>
+      <c r="AB23" s="124"/>
       <c r="AC23" s="30"/>
       <c r="AD23" s="30"/>
       <c r="AE23" s="30"/>
@@ -6343,18 +6336,18 @@
     <row r="24" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="101">
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="99">
         <f>MAX(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I24" s="102"/>
+      <c r="I24" s="100"/>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
@@ -6380,12 +6373,12 @@
       <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
-      <c r="W24" s="106"/>
-      <c r="X24" s="107"/>
-      <c r="Y24" s="107"/>
-      <c r="Z24" s="108"/>
-      <c r="AA24" s="111"/>
-      <c r="AB24" s="112"/>
+      <c r="W24" s="120"/>
+      <c r="X24" s="121"/>
+      <c r="Y24" s="121"/>
+      <c r="Z24" s="122"/>
+      <c r="AA24" s="125"/>
+      <c r="AB24" s="126"/>
       <c r="AC24" s="30"/>
       <c r="AD24" s="30"/>
       <c r="AE24" s="30"/>
@@ -7194,7 +7187,7 @@
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="30"/>
-      <c r="I42" s="115"/>
+      <c r="I42" s="46"/>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
       <c r="L42" s="30"/>
@@ -7325,12 +7318,12 @@
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="116"/>
-      <c r="E45" s="116"/>
-      <c r="F45" s="116"/>
-      <c r="G45" s="116"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
       <c r="H45" s="30"/>
       <c r="I45" s="30"/>
       <c r="J45" s="30"/>
@@ -7371,12 +7364,12 @@
     </row>
     <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
-      <c r="B46" s="117"/>
-      <c r="C46" s="117"/>
-      <c r="D46" s="117"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="117"/>
-      <c r="G46" s="117"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
@@ -7968,17 +7961,41 @@
       <c r="AR58" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="AA21:AB22"/>
-    <mergeCell ref="W21:Z22"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="Q20:S20"/>
+  <mergeCells count="57">
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="W23:Z24"/>
+    <mergeCell ref="AA23:AB24"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="C19:G19"/>
@@ -7991,43 +8008,17 @@
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="L15:P15"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="X18:Z18"/>
     <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L16:P16"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="W23:Z24"/>
-    <mergeCell ref="AA23:AB24"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="AA21:AB22"/>
+    <mergeCell ref="W21:Z22"/>
   </mergeCells>
   <conditionalFormatting sqref="W6:AB11 H18:H21 H23:H24 AA13:AA15 AA17:AA18">
     <cfRule type="colorScale" priority="12">
@@ -8101,7 +8092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M6:R11 Q15:Q16">
+  <conditionalFormatting sqref="M6:R11 Q13:Q14">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8113,7 +8104,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
+  <conditionalFormatting sqref="Q15">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="5"/>
@@ -8162,6 +8153,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed complete response time bug (mostly)
</commit_message>
<xml_diff>
--- a/Results Template.xlsx
+++ b/Results Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\$Current Projects\Response Time Tool\OSRTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\$Current Projects\Response Time Tool\OSRTT\OSRTT Launcher\OSRTT Launcher\bin\Release\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>Starting RGB</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Input Lag (ms)</t>
+  </si>
+  <si>
+    <t>Total System Latency (ms)</t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1018,12 +1021,30 @@
     <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1060,26 +1081,62 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1090,12 +1147,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1118,142 +1241,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2473,13 +2476,13 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2487,13 +2490,13 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -2501,13 +2504,13 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="50" t="s">
+      <c r="Z2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
@@ -2557,14 +2560,14 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
+      <c r="D4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="4"/>
       <c r="K4" s="8" t="s">
         <v>3</v>
@@ -2575,14 +2578,14 @@
       <c r="M4" s="4"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
+      <c r="P4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
       <c r="V4" s="4"/>
       <c r="W4" s="8" t="s">
         <v>3</v>
@@ -2594,14 +2597,14 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
+      <c r="AB4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
+      <c r="AG4" s="51"/>
       <c r="AH4" s="4"/>
       <c r="AI4" s="8" t="s">
         <v>3</v>
@@ -2720,7 +2723,7 @@
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
@@ -2757,7 +2760,7 @@
         <v>100</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="51" t="s">
+      <c r="N6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="1">
@@ -2794,7 +2797,7 @@
         <v>100</v>
       </c>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="51" t="s">
+      <c r="Z6" s="56" t="s">
         <v>2</v>
       </c>
       <c r="AA6" s="1">
@@ -2833,7 +2836,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="51"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2863,7 +2866,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="51"/>
+      <c r="N7" s="56"/>
       <c r="O7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2893,7 +2896,7 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="51"/>
+      <c r="Z7" s="56"/>
       <c r="AA7" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -2925,7 +2928,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="51"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -2960,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="51"/>
+      <c r="N8" s="56"/>
       <c r="O8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -2995,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="51"/>
+      <c r="Z8" s="56"/>
       <c r="AA8" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -3032,7 +3035,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="51"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3067,7 +3070,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="51"/>
+      <c r="N9" s="56"/>
       <c r="O9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3102,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="51"/>
+      <c r="Z9" s="56"/>
       <c r="AA9" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -3139,7 +3142,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="51"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3174,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="51"/>
+      <c r="N10" s="56"/>
       <c r="O10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3209,7 +3212,7 @@
         <v>1</v>
       </c>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="51"/>
+      <c r="Z10" s="56"/>
       <c r="AA10" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -3246,7 +3249,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="51"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3281,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="3"/>
-      <c r="N11" s="51"/>
+      <c r="N11" s="56"/>
       <c r="O11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3316,7 +3319,7 @@
         <v>2</v>
       </c>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="51"/>
+      <c r="Z11" s="56"/>
       <c r="AA11" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -3599,13 +3602,13 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -3613,13 +3616,13 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="50" t="s">
+      <c r="N19" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
       <c r="S19" s="1"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -3659,14 +3662,14 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
+      <c r="D21" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
       <c r="J21" s="4"/>
       <c r="K21" s="8" t="s">
         <v>15</v>
@@ -3677,14 +3680,14 @@
       <c r="M21" s="4"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="50"/>
+      <c r="P21" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
       <c r="V21" s="4"/>
       <c r="W21" s="8" t="s">
         <v>3</v>
@@ -3694,15 +3697,15 @@
         <v>60</v>
       </c>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="56" t="s">
+      <c r="Z21" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="58"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="57"/>
+      <c r="AA21" s="64"/>
+      <c r="AB21" s="64"/>
+      <c r="AC21" s="64"/>
+      <c r="AD21" s="64"/>
+      <c r="AE21" s="64"/>
+      <c r="AF21" s="63"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -3771,23 +3774,23 @@
         <v>16.666666666666668</v>
       </c>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="56" t="s">
+      <c r="Z22" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="AA22" s="58"/>
-      <c r="AB22" s="58"/>
-      <c r="AC22" s="57"/>
-      <c r="AD22" s="56" t="s">
+      <c r="AA22" s="64"/>
+      <c r="AB22" s="64"/>
+      <c r="AC22" s="63"/>
+      <c r="AD22" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="AE22" s="57"/>
+      <c r="AE22" s="63"/>
       <c r="AF22" s="41" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="1">
@@ -3824,7 +3827,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="3"/>
-      <c r="N23" s="51" t="s">
+      <c r="N23" s="56" t="s">
         <v>2</v>
       </c>
       <c r="O23" s="1">
@@ -3861,16 +3864,16 @@
         <v>100</v>
       </c>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="59" t="s">
+      <c r="Z23" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="AA23" s="60"/>
-      <c r="AB23" s="60"/>
-      <c r="AC23" s="61"/>
-      <c r="AD23" s="62">
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="66"/>
+      <c r="AC23" s="67"/>
+      <c r="AD23" s="68">
         <v>0.33</v>
       </c>
-      <c r="AE23" s="61"/>
+      <c r="AE23" s="67"/>
       <c r="AF23" s="42">
         <f>100-$X$26</f>
         <v>99</v>
@@ -3878,7 +3881,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="51"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -3913,7 +3916,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="3"/>
-      <c r="N24" s="51"/>
+      <c r="N24" s="56"/>
       <c r="O24" s="1">
         <f>'PASTE DATA HERE'!$A$3</f>
         <v>51</v>
@@ -3943,16 +3946,16 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="68" t="s">
+      <c r="Z24" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="AA24" s="50"/>
-      <c r="AB24" s="50"/>
-      <c r="AC24" s="64"/>
-      <c r="AD24" s="63">
+      <c r="AA24" s="51"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="52"/>
+      <c r="AD24" s="69">
         <v>0.33</v>
       </c>
-      <c r="AE24" s="64"/>
+      <c r="AE24" s="52"/>
       <c r="AF24" s="43">
         <f>100-$L$9</f>
         <v>99</v>
@@ -3960,7 +3963,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="51"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -3995,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="3"/>
-      <c r="N25" s="51"/>
+      <c r="N25" s="56"/>
       <c r="O25" s="1">
         <f>'PASTE DATA HERE'!$A$5</f>
         <v>102</v>
@@ -4030,16 +4033,16 @@
         <v>1</v>
       </c>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="68" t="s">
+      <c r="Z25" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="AA25" s="50"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="64"/>
-      <c r="AD25" s="63">
+      <c r="AA25" s="51"/>
+      <c r="AB25" s="51"/>
+      <c r="AC25" s="52"/>
+      <c r="AD25" s="69">
         <v>0.1</v>
       </c>
-      <c r="AE25" s="64"/>
+      <c r="AE25" s="52"/>
       <c r="AF25" s="43">
         <f>100-$L$10</f>
         <v>99</v>
@@ -4047,7 +4050,7 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="51"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -4077,7 +4080,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="51"/>
+      <c r="N26" s="56"/>
       <c r="O26" s="1">
         <f>'PASTE DATA HERE'!$A$7</f>
         <v>153</v>
@@ -4112,16 +4115,16 @@
         <v>1</v>
       </c>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="68" t="s">
+      <c r="Z26" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="AA26" s="50"/>
-      <c r="AB26" s="50"/>
-      <c r="AC26" s="64"/>
-      <c r="AD26" s="63">
+      <c r="AA26" s="51"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="52"/>
+      <c r="AD26" s="69">
         <v>0.1</v>
       </c>
-      <c r="AE26" s="64"/>
+      <c r="AE26" s="52"/>
       <c r="AF26" s="43">
         <f>100-$L$11</f>
         <v>99</v>
@@ -4129,7 +4132,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="51"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -4159,7 +4162,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="51"/>
+      <c r="N27" s="56"/>
       <c r="O27" s="1">
         <f>'PASTE DATA HERE'!$A$9</f>
         <v>204</v>
@@ -4194,16 +4197,16 @@
         <v>1</v>
       </c>
       <c r="Y27" s="3"/>
-      <c r="Z27" s="68" t="s">
+      <c r="Z27" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="AA27" s="50"/>
-      <c r="AB27" s="50"/>
-      <c r="AC27" s="64"/>
-      <c r="AD27" s="63">
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="69">
         <v>0.1</v>
       </c>
-      <c r="AE27" s="64"/>
+      <c r="AE27" s="52"/>
       <c r="AF27" s="43">
         <f>100-$L$23</f>
         <v>99</v>
@@ -4211,7 +4214,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="51"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -4241,7 +4244,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="51"/>
+      <c r="N28" s="56"/>
       <c r="O28" s="1">
         <f>'PASTE DATA HERE'!$A$11</f>
         <v>255</v>
@@ -4276,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="69" t="s">
+      <c r="Z28" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="AA28" s="70"/>
-      <c r="AB28" s="70"/>
-      <c r="AC28" s="66"/>
-      <c r="AD28" s="65">
+      <c r="AA28" s="54"/>
+      <c r="AB28" s="54"/>
+      <c r="AC28" s="55"/>
+      <c r="AD28" s="70">
         <v>0.04</v>
       </c>
-      <c r="AE28" s="66"/>
+      <c r="AE28" s="55"/>
       <c r="AF28" s="44">
         <f>100-$L$5</f>
         <v>83.333333333333329</v>
@@ -4322,11 +4325,11 @@
         <v>2</v>
       </c>
       <c r="Y29" s="6"/>
-      <c r="AC29" s="53" t="s">
+      <c r="AC29" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="AD29" s="54"/>
-      <c r="AE29" s="55"/>
+      <c r="AD29" s="60"/>
+      <c r="AE29" s="61"/>
       <c r="AF29" s="45">
         <f>(($AF$23*$AD$23)+($AF$24*$AD$24)+($AF$25*$AD$25)+($AF$26*$AD$26)+($AF$27*$AD$27)+($AF$28*$AD$28))/10</f>
         <v>9.8373333333333353</v>
@@ -4398,23 +4401,23 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="67" t="s">
+      <c r="F32" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
       <c r="I32" s="12"/>
-      <c r="J32" s="52" t="s">
+      <c r="J32" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
       <c r="M32" s="6"/>
       <c r="N32" s="5"/>
       <c r="O32" s="1"/>
@@ -4557,24 +4560,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z25:AC25"/>
-    <mergeCell ref="Z26:AC26"/>
-    <mergeCell ref="Z27:AC27"/>
-    <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="P21:U21"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="N23:N28"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="N6:N11"/>
     <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AB4:AG4"/>
     <mergeCell ref="Z6:Z11"/>
@@ -4591,6 +4576,24 @@
     <mergeCell ref="AD26:AE26"/>
     <mergeCell ref="AD27:AE27"/>
     <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="P21:U21"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="N23:N28"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="Z24:AC24"/>
+    <mergeCell ref="Z25:AC25"/>
+    <mergeCell ref="Z26:AC26"/>
+    <mergeCell ref="Z27:AC27"/>
+    <mergeCell ref="Z28:AC28"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:I11 P6:U11 P23:U28 L8:L11 L13:L14 X8:X10 X12:X13 X25:X28 X30:X31">
     <cfRule type="colorScale" priority="10">
@@ -4628,7 +4631,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X11 L12 X29">
+  <conditionalFormatting sqref="L12 X11 X29">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="5"/>
@@ -4640,7 +4643,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X6 L6 X23">
+  <conditionalFormatting sqref="L6 X6 X23">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="50"/>
@@ -4735,7 +4738,7 @@
   <dimension ref="A1:AR58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AD29" sqref="AD29"/>
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4799,42 +4802,42 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
-      <c r="B2" s="108" t="str">
+      <c r="B2" s="74" t="str">
         <f>'PASTE DATA HERE'!$E$1</f>
         <v>Perceived Response Time - RGB5 (ms)</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="110"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
       <c r="J2" s="31"/>
-      <c r="K2" s="108" t="str">
+      <c r="K2" s="74" t="str">
         <f>'PASTE DATA HERE'!$F$1</f>
         <v>Overshoot (RGB)</v>
       </c>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="110"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="76"/>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
-      <c r="U2" s="108" t="str">
+      <c r="U2" s="74" t="str">
         <f>'PASTE DATA HERE'!$G$1</f>
         <v>Visual Response Rating</v>
       </c>
-      <c r="V2" s="109"/>
-      <c r="W2" s="109"/>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="110"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="76"/>
       <c r="AC2" s="31"/>
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
@@ -4902,37 +4905,37 @@
       <c r="A4" s="30"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
-      <c r="D4" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="57"/>
+      <c r="D4" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="63"/>
       <c r="J4" s="32"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
-      <c r="M4" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="57"/>
+      <c r="M4" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="63"/>
       <c r="S4" s="32"/>
       <c r="T4" s="30"/>
       <c r="U4" s="31"/>
       <c r="V4" s="31"/>
-      <c r="W4" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="57"/>
+      <c r="W4" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="63"/>
       <c r="AC4" s="32"/>
       <c r="AD4" s="34"/>
       <c r="AE4" s="33"/>
@@ -5052,7 +5055,7 @@
     </row>
     <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="71" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="25">
@@ -5081,7 +5084,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="33"/>
-      <c r="K6" s="114" t="s">
+      <c r="K6" s="71" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="25">
@@ -5111,7 +5114,7 @@
       </c>
       <c r="S6" s="33"/>
       <c r="T6" s="30"/>
-      <c r="U6" s="114" t="s">
+      <c r="U6" s="71" t="s">
         <v>2</v>
       </c>
       <c r="V6" s="25">
@@ -5158,7 +5161,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="115"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5185,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="33"/>
-      <c r="K7" s="115"/>
+      <c r="K7" s="72"/>
       <c r="L7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5213,7 +5216,7 @@
       </c>
       <c r="S7" s="33"/>
       <c r="T7" s="30"/>
-      <c r="U7" s="115"/>
+      <c r="U7" s="72"/>
       <c r="V7" s="26">
         <f>'PASTE DATA HERE'!$B$2</f>
         <v>51</v>
@@ -5258,7 +5261,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="115"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5285,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="33"/>
-      <c r="K8" s="115"/>
+      <c r="K8" s="72"/>
       <c r="L8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5313,7 +5316,7 @@
       </c>
       <c r="S8" s="33"/>
       <c r="T8" s="30"/>
-      <c r="U8" s="115"/>
+      <c r="U8" s="72"/>
       <c r="V8" s="26">
         <f>'PASTE DATA HERE'!$B$4</f>
         <v>102</v>
@@ -5358,7 +5361,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
-      <c r="B9" s="115"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5385,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="33"/>
-      <c r="K9" s="115"/>
+      <c r="K9" s="72"/>
       <c r="L9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5413,7 +5416,7 @@
       </c>
       <c r="S9" s="33"/>
       <c r="T9" s="33"/>
-      <c r="U9" s="115"/>
+      <c r="U9" s="72"/>
       <c r="V9" s="26">
         <f>'PASTE DATA HERE'!$B$6</f>
         <v>153</v>
@@ -5458,7 +5461,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="115"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5485,7 +5488,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="33"/>
-      <c r="K10" s="115"/>
+      <c r="K10" s="72"/>
       <c r="L10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5513,7 +5516,7 @@
       </c>
       <c r="S10" s="33"/>
       <c r="T10" s="33"/>
-      <c r="U10" s="115"/>
+      <c r="U10" s="72"/>
       <c r="V10" s="26">
         <f>'PASTE DATA HERE'!$B$8</f>
         <v>204</v>
@@ -5558,7 +5561,7 @@
     </row>
     <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
-      <c r="B11" s="116"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5585,7 +5588,7 @@
       </c>
       <c r="I11" s="24"/>
       <c r="J11" s="33"/>
-      <c r="K11" s="116"/>
+      <c r="K11" s="73"/>
       <c r="L11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5613,7 +5616,7 @@
       <c r="R11" s="24"/>
       <c r="S11" s="33"/>
       <c r="T11" s="33"/>
-      <c r="U11" s="116"/>
+      <c r="U11" s="73"/>
       <c r="V11" s="27">
         <f>'PASTE DATA HERE'!$B$10</f>
         <v>255</v>
@@ -5705,47 +5708,47 @@
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="103">
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="107">
         <f>'VIEW HEATMAPS HERE'!L4</f>
         <v>60</v>
       </c>
-      <c r="I13" s="104"/>
+      <c r="I13" s="108"/>
       <c r="J13" s="33"/>
       <c r="K13" s="30"/>
-      <c r="L13" s="89" t="s">
+      <c r="L13" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="92">
+      <c r="M13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="83">
         <f>AVERAGE(M6:R11)</f>
         <v>1</v>
       </c>
-      <c r="R13" s="93"/>
+      <c r="R13" s="84"/>
       <c r="S13" s="30"/>
       <c r="T13" s="30"/>
       <c r="U13" s="30"/>
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
-      <c r="X13" s="89" t="s">
+      <c r="X13" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="91"/>
-      <c r="AA13" s="92">
+      <c r="Y13" s="88"/>
+      <c r="Z13" s="104"/>
+      <c r="AA13" s="83">
         <f>AVERAGE(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB13" s="93"/>
+      <c r="AB13" s="84"/>
       <c r="AC13" s="30"/>
       <c r="AD13" s="30"/>
       <c r="AE13" s="30"/>
@@ -5766,47 +5769,47 @@
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="105">
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="109">
         <f>1000/$H$13</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="I14" s="106"/>
+      <c r="I14" s="110"/>
       <c r="J14" s="33"/>
       <c r="K14" s="30"/>
-      <c r="L14" s="71" t="s">
+      <c r="L14" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="101">
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="85">
         <f>MAX(M6:R11)</f>
         <v>1</v>
       </c>
-      <c r="R14" s="102"/>
+      <c r="R14" s="86"/>
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
-      <c r="X14" s="71" t="s">
+      <c r="X14" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="72"/>
-      <c r="Z14" s="73"/>
-      <c r="AA14" s="94">
+      <c r="Y14" s="90"/>
+      <c r="Z14" s="91"/>
+      <c r="AA14" s="105">
         <f>AVERAGE(X6:AB6,Y7:AB7,Z8:AB8,AA9:AB9,AB10)</f>
         <v>1</v>
       </c>
-      <c r="AB14" s="95"/>
+      <c r="AB14" s="106"/>
       <c r="AC14" s="30"/>
       <c r="AD14" s="30"/>
       <c r="AE14" s="30"/>
@@ -5827,47 +5830,47 @@
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="127">
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="111">
         <f>((COUNTIF(D6:I11, "&lt;" &amp;H14))/COUNT(D6:I11))*100</f>
         <v>100</v>
       </c>
-      <c r="I15" s="128"/>
+      <c r="I15" s="112"/>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="74" t="s">
+      <c r="L15" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="77">
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="114"/>
+      <c r="P15" s="116"/>
+      <c r="Q15" s="117">
         <f>((COUNTIF(M6:R11, "&gt;15"))/COUNT(M6:R11))*100</f>
         <v>0</v>
       </c>
-      <c r="R15" s="78"/>
+      <c r="R15" s="118"/>
       <c r="S15" s="30"/>
       <c r="T15" s="30"/>
       <c r="U15" s="30"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
-      <c r="X15" s="71" t="s">
+      <c r="X15" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="Y15" s="72"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="94">
+      <c r="Y15" s="90"/>
+      <c r="Z15" s="91"/>
+      <c r="AA15" s="105">
         <f>AVERAGE(W7:W11,X8:X11,Y9:Y11,Z10:Z11,AA11)</f>
         <v>1</v>
       </c>
-      <c r="AB15" s="95"/>
+      <c r="AB15" s="106"/>
       <c r="AC15" s="30"/>
       <c r="AD15" s="30"/>
       <c r="AE15" s="30"/>
@@ -5909,16 +5912,16 @@
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
-      <c r="X16" s="71" t="s">
+      <c r="X16" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="Y16" s="72"/>
-      <c r="Z16" s="73"/>
-      <c r="AA16" s="101">
+      <c r="Y16" s="90"/>
+      <c r="Z16" s="91"/>
+      <c r="AA16" s="85">
         <f>AB6+W11</f>
         <v>2</v>
       </c>
-      <c r="AB16" s="102"/>
+      <c r="AB16" s="86"/>
       <c r="AC16" s="30"/>
       <c r="AD16" s="30"/>
       <c r="AE16" s="30"/>
@@ -5939,18 +5942,18 @@
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="92">
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="83">
         <f>'VIEW HEATMAPS HERE'!$X$26</f>
         <v>1</v>
       </c>
-      <c r="I17" s="93"/>
+      <c r="I17" s="84"/>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
@@ -5965,16 +5968,16 @@
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
       <c r="W17" s="30"/>
-      <c r="X17" s="71" t="s">
+      <c r="X17" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="Y17" s="72"/>
-      <c r="Z17" s="73"/>
-      <c r="AA17" s="101">
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="91"/>
+      <c r="AA17" s="85">
         <f>MIN(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB17" s="102"/>
+      <c r="AB17" s="86"/>
       <c r="AC17" s="30"/>
       <c r="AD17" s="30"/>
       <c r="AE17" s="30"/>
@@ -5995,18 +5998,18 @@
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="94">
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="105">
         <f>'VIEW HEATMAPS HERE'!$X$8</f>
         <v>1</v>
       </c>
-      <c r="I18" s="95"/>
+      <c r="I18" s="106"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -6021,16 +6024,16 @@
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
-      <c r="X18" s="74" t="s">
+      <c r="X18" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="Y18" s="75"/>
-      <c r="Z18" s="76"/>
-      <c r="AA18" s="99">
+      <c r="Y18" s="114"/>
+      <c r="Z18" s="116"/>
+      <c r="AA18" s="92">
         <f>MAX(W6:AB11)</f>
         <v>1</v>
       </c>
-      <c r="AB18" s="100"/>
+      <c r="AB18" s="93"/>
       <c r="AC18" s="30"/>
       <c r="AD18" s="30"/>
       <c r="AE18" s="30"/>
@@ -6051,18 +6054,18 @@
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="30"/>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="94">
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="105">
         <f>AVERAGE(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I19" s="95"/>
+      <c r="I19" s="106"/>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -6102,32 +6105,32 @@
     <row r="20" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="30"/>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="94">
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="105">
         <f>AVERAGE(E6:I6,F7:I7,G8:I8,H9:I9,I10)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="95"/>
+      <c r="I20" s="106"/>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
-      <c r="M20" s="111" t="s">
+      <c r="M20" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="112"/>
-      <c r="O20" s="113"/>
+      <c r="N20" s="78"/>
+      <c r="O20" s="79"/>
       <c r="P20" s="30"/>
-      <c r="Q20" s="96" t="s">
+      <c r="Q20" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="R20" s="97"/>
-      <c r="S20" s="98"/>
+      <c r="R20" s="81"/>
+      <c r="S20" s="82"/>
       <c r="T20" s="30"/>
       <c r="U20" s="30"/>
       <c r="V20" s="30"/>
@@ -6157,18 +6160,18 @@
     <row r="21" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="94">
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="105">
         <f>AVERAGE(D7:D11,E8:E11,F9:F11,G10:G11,H11)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="95"/>
+      <c r="I21" s="106"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -6194,17 +6197,17 @@
       <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="1"/>
-      <c r="W21" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="X21" s="84"/>
-      <c r="Y21" s="84"/>
-      <c r="Z21" s="85"/>
-      <c r="AA21" s="79">
+      <c r="W21" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="X21" s="124"/>
+      <c r="Y21" s="124"/>
+      <c r="Z21" s="125"/>
+      <c r="AA21" s="119">
         <f>AVERAGE('PASTE DATA HERE'!H2:H31)</f>
         <v>1</v>
       </c>
-      <c r="AB21" s="80"/>
+      <c r="AB21" s="120"/>
       <c r="AC21" s="30"/>
       <c r="AD21" s="30"/>
       <c r="AE21" s="30"/>
@@ -6225,18 +6228,18 @@
     <row r="22" spans="1:44" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30"/>
       <c r="B22" s="30"/>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="101">
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="85">
         <f>I6+D11</f>
         <v>2</v>
       </c>
-      <c r="I22" s="102"/>
+      <c r="I22" s="86"/>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
@@ -6250,12 +6253,12 @@
       <c r="T22" s="30"/>
       <c r="U22" s="30"/>
       <c r="V22" s="49"/>
-      <c r="W22" s="86"/>
-      <c r="X22" s="87"/>
-      <c r="Y22" s="87"/>
-      <c r="Z22" s="88"/>
-      <c r="AA22" s="81"/>
-      <c r="AB22" s="82"/>
+      <c r="W22" s="126"/>
+      <c r="X22" s="127"/>
+      <c r="Y22" s="127"/>
+      <c r="Z22" s="128"/>
+      <c r="AA22" s="121"/>
+      <c r="AB22" s="122"/>
       <c r="AC22" s="30"/>
       <c r="AD22" s="30"/>
       <c r="AE22" s="30"/>
@@ -6276,46 +6279,46 @@
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="101">
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="85">
         <f>MIN(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I23" s="102"/>
+      <c r="I23" s="86"/>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="96" t="s">
+      <c r="M23" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="97"/>
-      <c r="O23" s="98"/>
+      <c r="N23" s="81"/>
+      <c r="O23" s="82"/>
       <c r="P23" s="30"/>
-      <c r="Q23" s="59" t="s">
+      <c r="Q23" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="R23" s="60"/>
-      <c r="S23" s="61"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="67"/>
       <c r="T23" s="30"/>
       <c r="U23" s="30"/>
       <c r="V23" s="30"/>
-      <c r="W23" s="117" t="s">
+      <c r="W23" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="X23" s="118"/>
-      <c r="Y23" s="118"/>
-      <c r="Z23" s="119"/>
-      <c r="AA23" s="123">
+      <c r="X23" s="95"/>
+      <c r="Y23" s="95"/>
+      <c r="Z23" s="96"/>
+      <c r="AA23" s="100">
         <f>'VIEW HEATMAPS HERE'!$AF$29</f>
         <v>9.8373333333333353</v>
       </c>
-      <c r="AB23" s="124"/>
+      <c r="AB23" s="101"/>
       <c r="AC23" s="30"/>
       <c r="AD23" s="30"/>
       <c r="AE23" s="30"/>
@@ -6336,18 +6339,18 @@
     <row r="24" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="74" t="s">
+      <c r="C24" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="99">
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="92">
         <f>MAX(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I24" s="100"/>
+      <c r="I24" s="93"/>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
@@ -6373,12 +6376,12 @@
       <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
-      <c r="W24" s="120"/>
-      <c r="X24" s="121"/>
-      <c r="Y24" s="121"/>
-      <c r="Z24" s="122"/>
-      <c r="AA24" s="125"/>
-      <c r="AB24" s="126"/>
+      <c r="W24" s="97"/>
+      <c r="X24" s="98"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="99"/>
+      <c r="AA24" s="102"/>
+      <c r="AB24" s="103"/>
       <c r="AC24" s="30"/>
       <c r="AD24" s="30"/>
       <c r="AE24" s="30"/>
@@ -7962,12 +7965,41 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="AA21:AB22"/>
+    <mergeCell ref="W21:Z22"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
     <mergeCell ref="Q23:S23"/>
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="M23:O23"/>
@@ -7981,44 +8013,15 @@
     <mergeCell ref="AA18:AB18"/>
     <mergeCell ref="W23:Z24"/>
     <mergeCell ref="AA23:AB24"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="Q20:S20"/>
     <mergeCell ref="L15:P15"/>
     <mergeCell ref="X17:Z17"/>
     <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="AA21:AB22"/>
-    <mergeCell ref="W21:Z22"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="W6:AB11 H18:H21 H23:H24 AA13:AA15 AA17:AA18">
     <cfRule type="colorScale" priority="12">

</xml_diff>

<commit_message>
Replaced Input Lag mode with DirectX Code. Added input lag results view. Added new tab to XLSX file. Fix monitor name failure. Moved input lag processing to processdata.
</commit_message>
<xml_diff>
--- a/Results Template.xlsx
+++ b/Results Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\$Current Projects\Response Time Tool\OSRTT\OSRTT Launcher\OSRTT Launcher\bin\Release\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\$Current Projects\Response Time Tool\OSRTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,14 +14,15 @@
   <sheets>
     <sheet name="PASTE DATA HERE" sheetId="1" r:id="rId1"/>
     <sheet name="VIEW HEATMAPS HERE" sheetId="2" r:id="rId2"/>
-    <sheet name="STANDARD RESULTS" sheetId="3" r:id="rId3"/>
+    <sheet name="RUNSTATS" sheetId="4" r:id="rId3"/>
+    <sheet name="STANDARD RESULTS" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
   <si>
     <t>Starting RGB</t>
   </si>
@@ -168,6 +169,15 @@
   </si>
   <si>
     <t>Total System Latency (ms)</t>
+  </si>
+  <si>
+    <t>Monitor Name</t>
+  </si>
+  <si>
+    <t>FPS Limit</t>
+  </si>
+  <si>
+    <t>VSYNC State</t>
   </si>
 </sst>
 </file>
@@ -1183,6 +1193,15 @@
     <xf numFmtId="2" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1210,16 +1229,7 @@
     <xf numFmtId="2" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4734,10 +4744,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AR58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
@@ -5708,18 +5753,18 @@
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="107" t="s">
+      <c r="C13" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="107">
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="110">
         <f>'VIEW HEATMAPS HERE'!L4</f>
         <v>60</v>
       </c>
-      <c r="I13" s="108"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="33"/>
       <c r="K13" s="30"/>
       <c r="L13" s="87" t="s">
@@ -5743,7 +5788,7 @@
         <v>32</v>
       </c>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="104"/>
+      <c r="Z13" s="107"/>
       <c r="AA13" s="83">
         <f>AVERAGE(W6:AB11)</f>
         <v>1</v>
@@ -5776,11 +5821,11 @@
       <c r="E14" s="90"/>
       <c r="F14" s="90"/>
       <c r="G14" s="90"/>
-      <c r="H14" s="109">
+      <c r="H14" s="112">
         <f>1000/$H$13</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="I14" s="110"/>
+      <c r="I14" s="113"/>
       <c r="J14" s="33"/>
       <c r="K14" s="30"/>
       <c r="L14" s="89" t="s">
@@ -5805,11 +5850,11 @@
       </c>
       <c r="Y14" s="90"/>
       <c r="Z14" s="91"/>
-      <c r="AA14" s="105">
+      <c r="AA14" s="108">
         <f>AVERAGE(X6:AB6,Y7:AB7,Z8:AB8,AA9:AB9,AB10)</f>
         <v>1</v>
       </c>
-      <c r="AB14" s="106"/>
+      <c r="AB14" s="109"/>
       <c r="AC14" s="30"/>
       <c r="AD14" s="30"/>
       <c r="AE14" s="30"/>
@@ -5830,27 +5875,27 @@
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
-      <c r="H15" s="111">
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="114">
         <f>((COUNTIF(D6:I11, "&lt;" &amp;H14))/COUNT(D6:I11))*100</f>
         <v>100</v>
       </c>
-      <c r="I15" s="112"/>
+      <c r="I15" s="115"/>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="113" t="s">
+      <c r="L15" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="114"/>
-      <c r="N15" s="114"/>
-      <c r="O15" s="114"/>
-      <c r="P15" s="116"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="106"/>
       <c r="Q15" s="117">
         <f>((COUNTIF(M6:R11, "&gt;15"))/COUNT(M6:R11))*100</f>
         <v>0</v>
@@ -5866,11 +5911,11 @@
       </c>
       <c r="Y15" s="90"/>
       <c r="Z15" s="91"/>
-      <c r="AA15" s="105">
+      <c r="AA15" s="108">
         <f>AVERAGE(W7:W11,X8:X11,Y9:Y11,Z10:Z11,AA11)</f>
         <v>1</v>
       </c>
-      <c r="AB15" s="106"/>
+      <c r="AB15" s="109"/>
       <c r="AC15" s="30"/>
       <c r="AD15" s="30"/>
       <c r="AE15" s="30"/>
@@ -5948,7 +5993,7 @@
       <c r="D17" s="88"/>
       <c r="E17" s="88"/>
       <c r="F17" s="88"/>
-      <c r="G17" s="104"/>
+      <c r="G17" s="107"/>
       <c r="H17" s="83">
         <f>'VIEW HEATMAPS HERE'!$X$26</f>
         <v>1</v>
@@ -6005,11 +6050,11 @@
       <c r="E18" s="90"/>
       <c r="F18" s="90"/>
       <c r="G18" s="91"/>
-      <c r="H18" s="105">
+      <c r="H18" s="108">
         <f>'VIEW HEATMAPS HERE'!$X$8</f>
         <v>1</v>
       </c>
-      <c r="I18" s="106"/>
+      <c r="I18" s="109"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -6024,11 +6069,11 @@
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
-      <c r="X18" s="113" t="s">
+      <c r="X18" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="Y18" s="114"/>
-      <c r="Z18" s="116"/>
+      <c r="Y18" s="105"/>
+      <c r="Z18" s="106"/>
       <c r="AA18" s="92">
         <f>MAX(W6:AB11)</f>
         <v>1</v>
@@ -6061,11 +6106,11 @@
       <c r="E19" s="90"/>
       <c r="F19" s="90"/>
       <c r="G19" s="91"/>
-      <c r="H19" s="105">
+      <c r="H19" s="108">
         <f>AVERAGE(D6:I11)</f>
         <v>1</v>
       </c>
-      <c r="I19" s="106"/>
+      <c r="I19" s="109"/>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
@@ -6112,11 +6157,11 @@
       <c r="E20" s="90"/>
       <c r="F20" s="90"/>
       <c r="G20" s="91"/>
-      <c r="H20" s="105">
+      <c r="H20" s="108">
         <f>AVERAGE(E6:I6,F7:I7,G8:I8,H9:I9,I10)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="106"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
@@ -6167,11 +6212,11 @@
       <c r="E21" s="90"/>
       <c r="F21" s="90"/>
       <c r="G21" s="91"/>
-      <c r="H21" s="105">
+      <c r="H21" s="108">
         <f>AVERAGE(D7:D11,E8:E11,F9:F11,G10:G11,H11)</f>
         <v>1</v>
       </c>
-      <c r="I21" s="106"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
@@ -6339,13 +6384,13 @@
     <row r="24" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="113" t="s">
+      <c r="C24" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="116"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="106"/>
       <c r="H24" s="92">
         <f>MAX(D6:I11)</f>
         <v>1</v>

</xml_diff>